<commit_message>
Changes for forecaster release 3.10.3
</commit_message>
<xml_diff>
--- a/schedules/Influenza.xlsx
+++ b/schedules/Influenza.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="304"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="358" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$145</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$94</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$94</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$146</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$95</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$95</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -93,9 +93,6 @@
     <t>Overdue</t>
   </si>
   <si>
-    <t>4 months</t>
-  </si>
-  <si>
     <t>influenza, whole</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>180, 203</t>
   </si>
   <si>
-    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203</t>
-  </si>
-  <si>
     <t>Against</t>
   </si>
   <si>
@@ -292,6 +286,12 @@
   </si>
   <si>
     <t>current season</t>
+  </si>
+  <si>
+    <t>5 months</t>
+  </si>
+  <si>
+    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 186, 187, 188, 189</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -488,11 +488,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="62"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="62"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="62"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="62"/>
+      </right>
+      <top style="thin">
+        <color indexed="62"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="62"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="62"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="62"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="62"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="62"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="62"/>
+      </left>
+      <right style="thin">
+        <color indexed="62"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="62"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -576,9 +651,42 @@
     <xf numFmtId="14" fontId="2" fillId="6" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -586,18 +694,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,13 +785,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>148167</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>592666</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>63049</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -719,7 +815,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="95249" y="5492750"/>
+          <a:off x="95249" y="5175250"/>
           <a:ext cx="6011334" cy="6106132"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1080,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IT146"/>
+  <dimension ref="A1:IT147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1124,296 +1220,293 @@
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="C4" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="43"/>
     </row>
     <row r="5" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="46"/>
+    </row>
+    <row r="6" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C7" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="41">
+        <v>82</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="37">
         <v>-503</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="37" t="s">
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="5" t="s">
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="15" t="s">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18">
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18">
         <v>2050</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="7">
-        <v>180</v>
-      </c>
-      <c r="F13" s="7">
-        <v>111</v>
-      </c>
-      <c r="H13" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="37"/>
+      <c r="F13" s="7"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
       <c r="E14" s="7">
+        <v>180</v>
+      </c>
+      <c r="F14" s="7">
+        <v>111</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="38"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="7">
         <v>181</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F15" s="7">
         <v>15</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H15" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I15" s="7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18">
-        <v>1430</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="H15" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="15" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="17"/>
       <c r="E16" s="18">
-        <v>1440</v>
+        <v>1430</v>
       </c>
       <c r="F16" s="7"/>
       <c r="H16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18">
+        <v>1440</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="H17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I17" s="7" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="7">
-        <v>179</v>
-      </c>
-      <c r="F17" s="7">
-        <v>88</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21"/>
       <c r="E18" s="7">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="F18" s="7">
-        <v>140</v>
+        <v>88</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
       <c r="E19" s="7">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F19" s="7">
-        <v>141</v>
-      </c>
-      <c r="I19" s="9"/>
+        <v>140</v>
+      </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21"/>
       <c r="E20" s="7">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="F20" s="7">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
       <c r="E21" s="7">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F21" s="7">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="21"/>
       <c r="E22" s="7">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F22" s="7">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
       <c r="E23" s="7">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F23" s="7">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
       <c r="E24" s="7">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F24" s="7">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="19"/>
+      <c r="B25" s="19" t="s">
+        <v>29</v>
+      </c>
       <c r="C25" s="20"/>
       <c r="D25" s="21"/>
       <c r="E25" s="7">
-        <v>204</v>
-      </c>
-      <c r="F25" s="7"/>
+        <v>189</v>
+      </c>
+      <c r="F25" s="7">
+        <v>127</v>
+      </c>
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
@@ -1421,7 +1514,7 @@
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
       <c r="E26" s="7">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F26" s="7"/>
       <c r="I26" s="9"/>
@@ -1430,11 +1523,18 @@
       <c r="B27" s="19"/>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
-      <c r="E27" s="7"/>
+      <c r="E27" s="7">
+        <v>203</v>
+      </c>
       <c r="F27" s="7"/>
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
@@ -1570,102 +1670,91 @@
       <c r="I72" s="9"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B73" s="10" t="s">
+      <c r="I73" s="9"/>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B74" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C74" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="D74" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D73" s="10" t="s">
+      <c r="E74" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B75" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E73" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="I73" s="9"/>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B74" s="23" t="s">
+      <c r="C75" s="23">
+        <v>1</v>
+      </c>
+      <c r="D75" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C74" s="23">
-        <v>1</v>
-      </c>
-      <c r="D74" s="23" t="s">
+      <c r="I75" s="9"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B76" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="I74" s="9"/>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B75" s="37" t="s">
+      <c r="C76" s="38"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="38"/>
+      <c r="I76" s="9"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B77" s="24"/>
+      <c r="C77" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C75" s="37"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="37"/>
-      <c r="I75" s="9"/>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B76" s="24"/>
-      <c r="C76" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D76" s="5" t="s">
+      <c r="E77" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I76" s="9"/>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B77" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="I77" s="9"/>
-      <c r="J77" s="9"/>
-      <c r="K77" s="25"/>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B78" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="I78" s="9"/>
       <c r="J78" s="9"/>
       <c r="K78" s="25"/>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B79" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>16</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
-      <c r="H79" s="25"/>
       <c r="I79" s="9"/>
       <c r="J79" s="9"/>
       <c r="K79" s="25"/>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B80" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
@@ -1676,10 +1765,10 @@
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" s="14" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
@@ -1689,13 +1778,13 @@
       <c r="K81" s="25"/>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B82" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C82" s="27"/>
-      <c r="D82" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="B82" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D82" s="7"/>
       <c r="E82" s="7"/>
       <c r="H82" s="25"/>
       <c r="I82" s="9"/>
@@ -1704,10 +1793,12 @@
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" s="26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C83" s="27"/>
-      <c r="D83" s="7"/>
+      <c r="D83" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="E83" s="7"/>
       <c r="H83" s="25"/>
       <c r="I83" s="9"/>
@@ -1715,112 +1806,111 @@
       <c r="K83" s="25"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B84" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C84" s="37"/>
-      <c r="D84" s="37"/>
+      <c r="B84" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C84" s="27"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
       <c r="H84" s="25"/>
       <c r="I84" s="9"/>
       <c r="J84" s="9"/>
       <c r="K84" s="25"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B85" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G85" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H85" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="B85" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
+      <c r="H85" s="25"/>
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
       <c r="K85" s="25"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B86" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
-      <c r="F86" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G86" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H86" s="7" t="s">
-        <v>68</v>
+      <c r="B86" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G86" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="I86" s="9"/>
       <c r="J86" s="9"/>
+      <c r="K86" s="25"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B87" s="37" t="s">
+      <c r="B87" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I87" s="9"/>
+      <c r="J87" s="9"/>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B88" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C88" s="38"/>
+      <c r="D88" s="38"/>
+      <c r="J88" s="9"/>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B89" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E89" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C87" s="37"/>
-      <c r="D87" s="37"/>
-      <c r="J87" s="9"/>
-    </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B88" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D88" s="5" t="s">
+      <c r="F89" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E88" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J88" s="9"/>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B89" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E89" s="7"/>
-      <c r="F89" s="8"/>
       <c r="J89" s="9"/>
-      <c r="K89" s="25"/>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D90" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="E90" s="7"/>
       <c r="F90" s="8"/>
       <c r="J90" s="9"/>
@@ -1828,10 +1918,10 @@
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" s="7" t="s">
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
@@ -1840,590 +1930,604 @@
       <c r="K91" s="25"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B92" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C92" s="7">
-        <v>1</v>
-      </c>
+      <c r="B92" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="8"/>
       <c r="J92" s="9"/>
       <c r="K92" s="25"/>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B93" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C93" s="7">
         <v>1</v>
       </c>
-      <c r="H93" s="25"/>
-      <c r="I93" s="9"/>
       <c r="J93" s="9"/>
       <c r="K93" s="25"/>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B94" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C94" s="7">
+        <v>1</v>
+      </c>
       <c r="H94" s="25"/>
       <c r="I94" s="9"/>
       <c r="J94" s="9"/>
       <c r="K94" s="25"/>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B95" s="10" t="s">
+      <c r="H95" s="25"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="25"/>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B96" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C96" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C95" s="10" t="s">
+      <c r="D96" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D95" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E95" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="F95" s="22"/>
-    </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B96" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C96" s="23">
+      <c r="E96" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="F96" s="22"/>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B97" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C97" s="23">
         <v>1</v>
       </c>
-      <c r="D96" s="23"/>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B97" s="37" t="s">
+      <c r="D97" s="23"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B98" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C98" s="38"/>
+      <c r="D98" s="38"/>
+      <c r="E98" s="38"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B99" s="24"/>
+      <c r="C99" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C97" s="37"/>
-      <c r="D97" s="37"/>
-      <c r="E97" s="37"/>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B98" s="24"/>
-      <c r="C98" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D98" s="5" t="s">
+      <c r="E99" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B99" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B100" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C100" s="7"/>
-      <c r="D100" s="7"/>
-      <c r="E100" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B101" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>16</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C101" s="7"/>
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B102" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B103" s="14" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B104" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C104" s="27"/>
-      <c r="D104" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E104" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="B104" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B105" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C105" s="27"/>
+      <c r="D105" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B106" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C106" s="27"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B107" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C105" s="27"/>
-      <c r="D105" s="7"/>
-      <c r="E105" s="7"/>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B106" s="37" t="s">
+      <c r="C107" s="38"/>
+      <c r="D107" s="38"/>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B108" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C106" s="37"/>
-      <c r="D106" s="37"/>
-    </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B107" s="5" t="s">
+      <c r="D108" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H108" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B109" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H109" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B110" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C110" s="38"/>
+      <c r="D110" s="38"/>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B111" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C107" s="5" t="s">
+      <c r="C111" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D111" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D107" s="5" t="s">
+      <c r="E111" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F111" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E107" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F107" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G107" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H107" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B108" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D108" s="7"/>
-      <c r="E108" s="7"/>
-      <c r="F108" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G108" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H108" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B109" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C109" s="37"/>
-      <c r="D109" s="37"/>
-    </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B110" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E110" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B111" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E111" s="7"/>
-      <c r="F111" s="8"/>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B112" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E112" s="7"/>
+      <c r="F112" s="8"/>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B113" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C112" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7" t="s">
+      <c r="C113" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F112" s="8"/>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B113" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C113" s="7">
-        <v>3</v>
-      </c>
+      <c r="F113" s="8"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B114" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C114" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B115" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C115" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B116" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B117" s="4" t="s">
-        <v>82</v>
+      <c r="B117" s="10" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B118" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="C118" s="37"/>
-      <c r="D118" s="37"/>
+      <c r="B118" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B119" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C119" s="38"/>
+      <c r="D119" s="38"/>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B120" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C120" s="50"/>
+      <c r="D120" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B121" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="C119" s="39"/>
-      <c r="D119" s="36" t="s">
+      <c r="C121" s="50"/>
+      <c r="D121" s="36" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B120" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="C120" s="39"/>
-      <c r="D120" s="36" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B121" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C121" s="13"/>
-      <c r="D121" s="36" t="s">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B122" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C122" s="13"/>
+      <c r="D122" s="36" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B122" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="C122" s="35"/>
-      <c r="D122" s="36" t="s">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B123" s="34" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B123" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="C123" s="37"/>
-      <c r="D123" s="37"/>
+      <c r="C123" s="35"/>
+      <c r="D123" s="36" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B124" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C124" s="39"/>
-      <c r="D124" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C124" s="38"/>
+      <c r="D124" s="38"/>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B125" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C125" s="50"/>
+      <c r="D125" s="36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B126" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C126" s="50"/>
+      <c r="D126" s="36" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B125" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C125" s="39"/>
-      <c r="D125" s="36" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B127" s="10" t="s">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B128" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C128" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C127" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E127" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="F127" s="22"/>
-    </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B128" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C128" s="23">
+      <c r="E128" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F128" s="22"/>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B129" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C129" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B129" s="37" t="s">
+    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B130" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C130" s="38"/>
+      <c r="D130" s="38"/>
+      <c r="E130" s="38"/>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B131" s="24"/>
+      <c r="C131" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D131" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C129" s="37"/>
-      <c r="D129" s="37"/>
-      <c r="E129" s="37"/>
-    </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B130" s="24"/>
-      <c r="C130" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D130" s="5" t="s">
+      <c r="E131" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E130" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B131" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C131" s="7"/>
-      <c r="D131" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E131" s="7"/>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B132" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C132" s="7"/>
-      <c r="D132" s="7"/>
+      <c r="D132" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="E132" s="7"/>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B133" s="14" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C133" s="7"/>
-      <c r="D133" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="D133" s="7"/>
       <c r="E133" s="7"/>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B134" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C134" s="7"/>
       <c r="D134" s="7" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="E134" s="7"/>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B135" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C135" s="7"/>
+      <c r="D135" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E135" s="7"/>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B136" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D136" s="7"/>
+      <c r="E136" s="7"/>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B137" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="C135" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D135" s="7"/>
-      <c r="E135" s="7"/>
-    </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B136" s="40" t="s">
+      <c r="C137" s="51"/>
+      <c r="D137" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C136" s="40"/>
-      <c r="D136" s="7" t="s">
+      <c r="E137" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B138" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E136" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B137" s="26" t="s">
+      <c r="C138" s="27"/>
+      <c r="D138" s="7"/>
+      <c r="E138" s="7"/>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B139" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C137" s="27"/>
-      <c r="D137" s="7"/>
-      <c r="E137" s="7"/>
-    </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B138" s="37" t="s">
+      <c r="C139" s="38"/>
+      <c r="D139" s="38"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B140" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C138" s="37"/>
-      <c r="D138" s="37"/>
-    </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B139" s="5" t="s">
+      <c r="D140" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G140" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H140" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B141" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
+      <c r="F141" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H141" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B142" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C142" s="38"/>
+      <c r="D142" s="38"/>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B143" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C139" s="5" t="s">
+      <c r="C143" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D143" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D139" s="5" t="s">
+      <c r="E143" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F143" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E139" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F139" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G139" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H139" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B140" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D140" s="7"/>
-      <c r="E140" s="7"/>
-      <c r="F140" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G140" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H140" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B141" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C141" s="37"/>
-      <c r="D141" s="37"/>
-    </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B142" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C142" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D142" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E142" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F142" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B143" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C143" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D143" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E143" s="7"/>
-      <c r="F143" s="8"/>
     </row>
     <row r="144" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B144" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D144" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="D144" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="E144" s="7"/>
       <c r="F144" s="8"/>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B145" s="14" t="s">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B145" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="8"/>
+    </row>
+    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B146" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C146" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B147" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C145" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B146" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C146" s="7">
+      <c r="C147" s="7">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="24">
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B75:E75"/>
+  <mergeCells count="25">
+    <mergeCell ref="B139:D139"/>
+    <mergeCell ref="B142:D142"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B98:E98"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="B110:D110"/>
+    <mergeCell ref="B130:E130"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B119:D119"/>
+    <mergeCell ref="B124:D124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B76:E76"/>
     <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="B138:D138"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B97:E97"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="B109:D109"/>
-    <mergeCell ref="B129:E129"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B118:D118"/>
-    <mergeCell ref="B123:D123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C4:F5"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2433,10 +2537,10 @@
     <oddFooter>&amp;CPrepared by  Nathan Bunker &amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <rowBreaks count="4" manualBreakCount="4">
-    <brk id="32" max="16383" man="1"/>
-    <brk id="72" max="16383" man="1"/>
-    <brk id="94" max="16383" man="1"/>
-    <brk id="126" max="16383" man="1"/>
+    <brk id="33" max="16383" man="1"/>
+    <brk id="73" max="16383" man="1"/>
+    <brk id="95" max="16383" man="1"/>
+    <brk id="127" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -2446,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B56"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2466,124 +2570,124 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 186, 187, 188, 189"/&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="29" t="str">
-        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B5&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C5&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Nasal" vaccineIds="180, 203"/&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="str">
-        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Live" vaccineIds="158, 159, 160, 161, 162, 171, 175, 178, 2020"/&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="29" t="str">
-        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B8&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C8&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="H1N1" vaccineIds="186, 187, 188, 189"/&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="29" t="str">
-        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B8&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C8&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B9&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C9&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Season Start" vaccineIds="-503"/&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="29" t="str">
-        <f>"  &lt;seasonal due="&amp;CHAR(34)&amp;Schedules!I16&amp;CHAR(34)&amp;" overdue="&amp;CHAR(34)&amp;Schedules!I17&amp;CHAR(34)&amp;" end="&amp;CHAR(34)&amp;Schedules!I15&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;seasonal due="1 month" overdue="4 months" end="6 months"/&gt;</v>
+        <f>"  &lt;seasonal due="&amp;CHAR(34)&amp;Schedules!I17&amp;CHAR(34)&amp;" overdue="&amp;CHAR(34)&amp;Schedules!I18&amp;CHAR(34)&amp;" end="&amp;CHAR(34)&amp;Schedules!I16&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">  &lt;seasonal due="1 month" overdue="5 months" end="6 months"/&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="29" t="str">
-        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B31&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C31&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D31&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B32&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C32&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D32&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;transition name="" age="" vaccineId=""/&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="str">
-        <f>Schedules!B74</f>
+        <f>Schedules!B75</f>
         <v>P1</v>
       </c>
       <c r="B9" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B74&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C74&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D74&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E73&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B75&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C75&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D75&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E74&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="season"&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C77&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D77&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E77&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C78&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D78&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E78&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C78&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D78&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E78&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C79&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D79&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E79&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C79&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D79&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E79&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B86&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F86&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G86&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H86&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B87&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C87&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D87&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E87&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F87&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G87&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H87&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B89&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C89&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F89&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E89&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B90&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C90&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F90&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B90&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C90&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F90&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B91&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C91&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D91&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F91&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E91&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B91&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C91&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D91&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F91&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E91&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B92&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F92&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Season Start" schedule="S1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
@@ -2595,77 +2699,77 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="str">
-        <f>Schedules!B96</f>
+        <f>Schedules!B97</f>
         <v>S1</v>
       </c>
       <c r="B23" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B96&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D96&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B97&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D97&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E96&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S1" dose="1" indication="" label="current season"&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="32" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C114&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C113&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C115&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C114&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="3"/&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C99&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D99&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E99&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D100&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E100&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D100&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E100&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D101&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E101&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D101&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E101&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C102&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D102&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E102&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C102&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D102&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E102&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B108&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C108&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F108&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G108&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H108&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B109&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C109&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E109&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F109&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G109&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H109&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B111&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C111&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D111&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F111&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E111&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B112&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C112&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F112&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E112&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B112&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C112&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F112&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E112&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B113&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C113&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D113&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F113&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E113&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="DL FLU 2014" age="" reason="" seasonCompleted="Yes"/&gt;</v>
       </c>
     </row>
@@ -2677,122 +2781,122 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="30" t="str">
-        <f>Schedules!B117</f>
+        <f>Schedules!B118</f>
         <v>DL FLU 2014</v>
       </c>
       <c r="B36" s="31" t="str">
-        <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B117&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B118&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;decisionLogic name="DL FLU 2014"&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" s="32" t="str">
-        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B119&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D119&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B120&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D120&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Season 2013 Start" value="07/01/2013"/&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="32" t="str">
-        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B120&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D120&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B121&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D121&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Season 2010 Start" value="07/01/2010"/&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="32" t="str">
-        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B121&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D121&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B122&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D122&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Flu"/&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B124&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D124&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B125&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D125&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Second Dose Needed" value="S2"/&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B125&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D125&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B126&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="No More Doses Needed" value="COMPLETE"/&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B42" s="32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="30" t="str">
-        <f>Schedules!B128</f>
+        <f>Schedules!B129</f>
         <v>S2</v>
       </c>
       <c r="B43" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B128&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C128&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D128&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E127&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B129&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C129&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D129&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E128&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S2" dose="2" indication="" label="2nd seasonal"&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C146&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C147&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C146&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C131&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D131&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E131&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E132&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E132&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="1 month" grace=""/&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B140&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C140&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D140&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E140&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F140&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G140&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H140&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B141&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C141&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D141&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E141&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F141&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G141&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H141&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B143&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C143&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D143&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F143&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H143&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E143&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B144&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F144&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H144&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E144&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B144&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F144&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H144&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E144&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B145&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D145&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F145&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H145&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E145&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="COMPLETE" age="" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Pneumo65 and Influenza for 2015
</commit_message>
<xml_diff>
--- a/schedules/Influenza.xlsx
+++ b/schedules/Influenza.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\forecast\forecaster2012\schedules\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="358"/>
+    <workbookView xWindow="14085" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$147</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$144</definedName>
     <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$96</definedName>
     <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$96</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="85">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -243,18 +238,6 @@
     <t>Decision Logic</t>
   </si>
   <si>
-    <t>Season 2013 Start</t>
-  </si>
-  <si>
-    <t>07/01/2013</t>
-  </si>
-  <si>
-    <t>Season 2010 Start</t>
-  </si>
-  <si>
-    <t>07/01/2010</t>
-  </si>
-  <si>
     <t>Constant Values</t>
   </si>
   <si>
@@ -267,9 +250,6 @@
     <t xml:space="preserve">  &lt;/decisionLogic&gt;</t>
   </si>
   <si>
-    <t>DL FLU 2014</t>
-  </si>
-  <si>
     <t>Valid Vaccine</t>
   </si>
   <si>
@@ -279,9 +259,6 @@
     <t>186, 187, 188, 189</t>
   </si>
   <si>
-    <t>Valid H1N1 Vaccine</t>
-  </si>
-  <si>
     <t>season</t>
   </si>
   <si>
@@ -295,13 +272,16 @@
   </si>
   <si>
     <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202</t>
+  </si>
+  <si>
+    <t>DL FLU 2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -570,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -645,12 +625,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="6" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -789,44 +763,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>346717</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>148167</xdr:rowOff>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>592666</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>63049</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>582084</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>121627</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="https://documents.lucidchart.com/documents/93c36fcd-5ce5-4343-a038-0b88849cce12/pages/0_0?a=4225&amp;x=167&amp;y=36&amp;w=935&amp;h=976&amp;store=1&amp;accept=image%2F*&amp;auth=LCA%201ccd8344df33cf5184460d1058691c59e7d5f632-ts%3D1435698127"/>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="95249" y="5175250"/>
-          <a:ext cx="6011334" cy="6106132"/>
+          <a:off x="1405050" y="5270500"/>
+          <a:ext cx="5939784" cy="6069460"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -877,7 +862,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -912,7 +897,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1101,11 +1086,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -1115,7 +1100,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1143,11 +1128,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -1157,7 +1142,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1174,21 +1159,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IT148"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IT145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="5" width="14.28515625" style="1" customWidth="1"/>
@@ -1212,8 +1197,8 @@
     <col min="23" max="254" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" ht="8.25" customHeight="1"/>
+    <row r="2" spans="2:9">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1222,89 +1207,89 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-    </row>
-    <row r="4" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="48" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+    </row>
+    <row r="4" spans="2:9" ht="12.75" customHeight="1">
+      <c r="B4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="44"/>
-    </row>
-    <row r="5" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="49"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47"/>
-    </row>
-    <row r="6" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
+    </row>
+    <row r="5" spans="2:9" ht="12.75" customHeight="1">
+      <c r="B5" s="47"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="45"/>
+    </row>
+    <row r="6" spans="2:9" ht="12.75" customHeight="1">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+    </row>
+    <row r="7" spans="2:9">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="36">
         <v>-503</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="39" t="s">
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+    </row>
+    <row r="12" spans="2:9">
       <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
@@ -1317,7 +1302,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9">
       <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
@@ -1329,7 +1314,7 @@
       <c r="F13" s="7"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9">
       <c r="B14" s="19" t="s">
         <v>17</v>
       </c>
@@ -1341,12 +1326,12 @@
       <c r="F14" s="7">
         <v>111</v>
       </c>
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="39"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I14" s="37"/>
+    </row>
+    <row r="15" spans="2:9">
       <c r="B15" s="19" t="s">
         <v>19</v>
       </c>
@@ -1365,7 +1350,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9">
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
@@ -1382,7 +1367,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9">
       <c r="B17" s="15" t="s">
         <v>22</v>
       </c>
@@ -1399,7 +1384,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9">
       <c r="B18" s="19" t="s">
         <v>1</v>
       </c>
@@ -1415,10 +1400,10 @@
         <v>21</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
       <c r="B19" s="19" t="s">
         <v>23</v>
       </c>
@@ -1431,7 +1416,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9">
       <c r="B20" s="19" t="s">
         <v>24</v>
       </c>
@@ -1445,7 +1430,7 @@
       </c>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9">
       <c r="B21" s="19" t="s">
         <v>25</v>
       </c>
@@ -1459,7 +1444,7 @@
       </c>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9">
       <c r="B22" s="19" t="s">
         <v>26</v>
       </c>
@@ -1473,7 +1458,7 @@
       </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9">
       <c r="B23" s="19" t="s">
         <v>27</v>
       </c>
@@ -1487,7 +1472,7 @@
       </c>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9">
       <c r="B24" s="19" t="s">
         <v>28</v>
       </c>
@@ -1501,7 +1486,7 @@
       </c>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9">
       <c r="B25" s="19" t="s">
         <v>29</v>
       </c>
@@ -1515,7 +1500,7 @@
       </c>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9">
       <c r="B26" s="19"/>
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
@@ -1525,7 +1510,7 @@
       <c r="F26" s="7"/>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9">
       <c r="B27" s="19"/>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
@@ -1535,9 +1520,9 @@
       <c r="F27" s="7"/>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9">
       <c r="B28" s="19" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="21"/>
@@ -1549,142 +1534,142 @@
       </c>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9">
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9">
       <c r="I30" s="9"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9">
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9">
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="9:9">
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="9:9">
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="9:9">
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="9:9">
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="9:9">
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="9:9">
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="9:9">
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="9:9">
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="9:9">
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="9:9">
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="9:9">
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="9:9">
       <c r="I44" s="9"/>
     </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="9:9">
       <c r="I45" s="9"/>
     </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="9:9">
       <c r="I46" s="9"/>
     </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="9:9">
       <c r="I47" s="9"/>
     </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="9:9">
       <c r="I48" s="9"/>
     </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="9:9">
       <c r="I49" s="9"/>
     </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="9:9">
       <c r="I50" s="9"/>
     </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="9:9">
       <c r="I51" s="9"/>
     </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="9:9">
       <c r="I52" s="9"/>
     </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="9:9">
       <c r="I53" s="9"/>
     </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="9:9">
       <c r="I54" s="9"/>
     </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="9:9">
       <c r="I55" s="9"/>
     </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="9:9">
       <c r="I56" s="9"/>
     </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="9:9">
       <c r="I57" s="9"/>
     </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="9:9">
       <c r="I58" s="9"/>
     </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="9:9">
       <c r="I59" s="9"/>
     </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="9:9">
       <c r="I60" s="9"/>
     </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="9:9">
       <c r="I61" s="9"/>
     </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="9:9">
       <c r="I62" s="9"/>
     </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="9:9">
       <c r="I63" s="9"/>
     </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="9:9">
       <c r="I64" s="9"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:11">
       <c r="I65" s="9"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:11">
       <c r="I66" s="9"/>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:11">
       <c r="I67" s="9"/>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:11">
       <c r="I68" s="9"/>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:11">
       <c r="I69" s="9"/>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:11">
       <c r="I70" s="9"/>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:11">
       <c r="I71" s="9"/>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:11">
       <c r="I72" s="9"/>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:11">
       <c r="I73" s="9"/>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:11">
       <c r="B74" s="10" t="s">
         <v>32</v>
       </c>
@@ -1695,11 +1680,11 @@
         <v>34</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I74" s="9"/>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:11">
       <c r="B75" s="23" t="s">
         <v>35</v>
       </c>
@@ -1711,16 +1696,16 @@
       </c>
       <c r="I75" s="9"/>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B76" s="39" t="s">
+    <row r="76" spans="2:11">
+      <c r="B76" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="39"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="39"/>
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
       <c r="I76" s="9"/>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:11">
       <c r="B77" s="24"/>
       <c r="C77" s="5" t="s">
         <v>31</v>
@@ -1733,7 +1718,7 @@
       </c>
       <c r="I77" s="9"/>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:11">
       <c r="B78" s="14" t="s">
         <v>40</v>
       </c>
@@ -1750,7 +1735,7 @@
       <c r="J78" s="9"/>
       <c r="K78" s="25"/>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:11">
       <c r="B79" s="14" t="s">
         <v>42</v>
       </c>
@@ -1761,7 +1746,7 @@
       <c r="J79" s="9"/>
       <c r="K79" s="25"/>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:11">
       <c r="B80" s="14" t="s">
         <v>20</v>
       </c>
@@ -1775,7 +1760,7 @@
       <c r="J80" s="9"/>
       <c r="K80" s="25"/>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:11">
       <c r="B81" s="14" t="s">
         <v>21</v>
       </c>
@@ -1789,7 +1774,7 @@
       <c r="J81" s="9"/>
       <c r="K81" s="25"/>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:11">
       <c r="B82" s="14" t="s">
         <v>44</v>
       </c>
@@ -1803,7 +1788,7 @@
       <c r="J82" s="9"/>
       <c r="K82" s="25"/>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:11">
       <c r="B83" s="26" t="s">
         <v>45</v>
       </c>
@@ -1817,7 +1802,7 @@
       <c r="J83" s="9"/>
       <c r="K83" s="25"/>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:11">
       <c r="B84" s="26" t="s">
         <v>47</v>
       </c>
@@ -1829,18 +1814,18 @@
       <c r="J84" s="9"/>
       <c r="K84" s="25"/>
     </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B85" s="39" t="s">
+    <row r="85" spans="2:11">
+      <c r="B85" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C85" s="39"/>
-      <c r="D85" s="39"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
       <c r="H85" s="25"/>
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
       <c r="K85" s="25"/>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:11">
       <c r="B86" s="5" t="s">
         <v>9</v>
       </c>
@@ -1866,7 +1851,7 @@
       <c r="J86" s="9"/>
       <c r="K86" s="25"/>
     </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:11">
       <c r="B87" s="7" t="s">
         <v>6</v>
       </c>
@@ -1887,15 +1872,15 @@
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
     </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B88" s="39" t="s">
+    <row r="88" spans="2:11">
+      <c r="B88" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C88" s="39"/>
-      <c r="D88" s="39"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="37"/>
       <c r="J88" s="9"/>
     </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:11">
       <c r="B89" s="5" t="s">
         <v>9</v>
       </c>
@@ -1913,7 +1898,7 @@
       </c>
       <c r="J89" s="9"/>
     </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:11">
       <c r="B90" s="7" t="s">
         <v>5</v>
       </c>
@@ -1928,7 +1913,7 @@
       <c r="J90" s="9"/>
       <c r="K90" s="25"/>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:11">
       <c r="B91" s="7" t="s">
         <v>4</v>
       </c>
@@ -1941,20 +1926,20 @@
       <c r="J91" s="9"/>
       <c r="K91" s="25"/>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:11">
       <c r="B92" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
-      <c r="F92" s="37"/>
+      <c r="F92" s="35"/>
       <c r="J92" s="9"/>
       <c r="K92" s="25"/>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:11">
       <c r="B93" s="7" t="s">
         <v>67</v>
       </c>
@@ -1967,7 +1952,7 @@
       <c r="J93" s="9"/>
       <c r="K93" s="25"/>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:11">
       <c r="B94" s="14" t="s">
         <v>57</v>
       </c>
@@ -1977,7 +1962,7 @@
       <c r="J94" s="9"/>
       <c r="K94" s="25"/>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:11">
       <c r="B95" s="14" t="s">
         <v>58</v>
       </c>
@@ -1989,13 +1974,13 @@
       <c r="J95" s="9"/>
       <c r="K95" s="25"/>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:11">
       <c r="H96" s="25"/>
       <c r="I96" s="9"/>
       <c r="J96" s="9"/>
       <c r="K96" s="25"/>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:8">
       <c r="B97" s="10" t="s">
         <v>32</v>
       </c>
@@ -2006,11 +1991,11 @@
         <v>34</v>
       </c>
       <c r="E97" s="22" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F97" s="22"/>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:8">
       <c r="B98" s="23" t="s">
         <v>56</v>
       </c>
@@ -2019,15 +2004,15 @@
       </c>
       <c r="D98" s="23"/>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B99" s="39" t="s">
+    <row r="99" spans="2:8">
+      <c r="B99" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C99" s="39"/>
-      <c r="D99" s="39"/>
-      <c r="E99" s="39"/>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C99" s="37"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
+    </row>
+    <row r="100" spans="2:8">
       <c r="B100" s="24"/>
       <c r="C100" s="5" t="s">
         <v>31</v>
@@ -2039,7 +2024,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:8">
       <c r="B101" s="14" t="s">
         <v>40</v>
       </c>
@@ -2053,7 +2038,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:8">
       <c r="B102" s="14" t="s">
         <v>42</v>
       </c>
@@ -2061,7 +2046,7 @@
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:8">
       <c r="B103" s="14" t="s">
         <v>20</v>
       </c>
@@ -2071,7 +2056,7 @@
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:8">
       <c r="B104" s="14" t="s">
         <v>21</v>
       </c>
@@ -2081,7 +2066,7 @@
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:8">
       <c r="B105" s="14" t="s">
         <v>44</v>
       </c>
@@ -2091,7 +2076,7 @@
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:8">
       <c r="B106" s="26" t="s">
         <v>45</v>
       </c>
@@ -2103,7 +2088,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:8">
       <c r="B107" s="26" t="s">
         <v>47</v>
       </c>
@@ -2111,14 +2096,14 @@
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B108" s="39" t="s">
+    <row r="108" spans="2:8">
+      <c r="B108" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C108" s="39"/>
-      <c r="D108" s="39"/>
-    </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C108" s="37"/>
+      <c r="D108" s="37"/>
+    </row>
+    <row r="109" spans="2:8">
       <c r="B109" s="5" t="s">
         <v>9</v>
       </c>
@@ -2141,7 +2126,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:8">
       <c r="B110" s="7" t="s">
         <v>6</v>
       </c>
@@ -2160,14 +2145,14 @@
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B111" s="39" t="s">
+    <row r="111" spans="2:8">
+      <c r="B111" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C111" s="39"/>
-      <c r="D111" s="39"/>
-    </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C111" s="37"/>
+      <c r="D111" s="37"/>
+    </row>
+    <row r="112" spans="2:8">
       <c r="B112" s="5" t="s">
         <v>9</v>
       </c>
@@ -2184,7 +2169,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:6">
       <c r="B113" s="7" t="s">
         <v>5</v>
       </c>
@@ -2197,12 +2182,12 @@
       <c r="E113" s="7"/>
       <c r="F113" s="8"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:6">
       <c r="B114" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D114" s="7"/>
       <c r="E114" s="7" t="s">
@@ -2210,7 +2195,7 @@
       </c>
       <c r="F114" s="8"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:6">
       <c r="B115" s="14" t="s">
         <v>57</v>
       </c>
@@ -2218,7 +2203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:6">
       <c r="B116" s="14" t="s">
         <v>58</v>
       </c>
@@ -2226,323 +2211,294 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:6">
       <c r="B118" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:6">
       <c r="B119" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B120" s="39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6">
+      <c r="B120" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C120" s="37"/>
+      <c r="D120" s="37"/>
+    </row>
+    <row r="121" spans="2:6">
+      <c r="B121" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C120" s="39"/>
-      <c r="D120" s="39"/>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B121" s="50" t="s">
-        <v>72</v>
-      </c>
-      <c r="C121" s="51"/>
-      <c r="D121" s="36" t="s">
+      <c r="C121" s="13"/>
+      <c r="D121" s="34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6">
+      <c r="B122" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C122" s="37"/>
+      <c r="D122" s="37"/>
+    </row>
+    <row r="123" spans="2:6">
+      <c r="B123" s="48" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B122" s="50" t="s">
+      <c r="C123" s="49"/>
+      <c r="D123" s="34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6">
+      <c r="B124" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="C122" s="51"/>
-      <c r="D122" s="36" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B123" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C123" s="13"/>
-      <c r="D123" s="36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B124" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="C124" s="35"/>
-      <c r="D124" s="36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B125" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C125" s="39"/>
-      <c r="D125" s="39"/>
-    </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B126" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="C126" s="51"/>
-      <c r="D126" s="36" t="s">
+      <c r="C124" s="49"/>
+      <c r="D124" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6">
+      <c r="B126" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C126" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E126" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F126" s="22"/>
+    </row>
+    <row r="127" spans="2:6">
+      <c r="B127" s="23" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B127" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="C127" s="51"/>
-      <c r="D127" s="36" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B129" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C129" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E129" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F129" s="22"/>
-    </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B130" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C130" s="23">
+      <c r="C127" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B131" s="39" t="s">
+    <row r="128" spans="2:6">
+      <c r="B128" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C131" s="39"/>
-      <c r="D131" s="39"/>
-      <c r="E131" s="39"/>
-    </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B132" s="24"/>
-      <c r="C132" s="5" t="s">
+      <c r="C128" s="37"/>
+      <c r="D128" s="37"/>
+      <c r="E128" s="37"/>
+    </row>
+    <row r="129" spans="2:8">
+      <c r="B129" s="24"/>
+      <c r="C129" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D129" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E132" s="5" t="s">
+      <c r="E129" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:8">
+      <c r="B130" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C130" s="7"/>
+      <c r="D130" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E130" s="7"/>
+    </row>
+    <row r="131" spans="2:8">
+      <c r="B131" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C131" s="7"/>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+    </row>
+    <row r="132" spans="2:8">
+      <c r="B132" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C132" s="7"/>
+      <c r="D132" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E132" s="7"/>
+    </row>
+    <row r="133" spans="2:8">
       <c r="B133" s="14" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C133" s="7"/>
       <c r="D133" s="7" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:8">
       <c r="B134" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C134" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="C134" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B135" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C135" s="7"/>
+    <row r="135" spans="2:8">
+      <c r="B135" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C135" s="50"/>
       <c r="D135" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E135" s="7"/>
-    </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B136" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C136" s="7"/>
-      <c r="D136" s="7" t="s">
-        <v>59</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E135" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8">
+      <c r="B136" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C136" s="27"/>
+      <c r="D136" s="7"/>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B137" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C137" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D137" s="7"/>
-      <c r="E137" s="7"/>
-    </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B138" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="C138" s="52"/>
-      <c r="D138" s="7" t="s">
+    <row r="137" spans="2:8">
+      <c r="B137" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C137" s="37"/>
+      <c r="D137" s="37"/>
+    </row>
+    <row r="138" spans="2:8">
+      <c r="B138" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G138" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H138" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="139" spans="2:8">
+      <c r="B139" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E138" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B139" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C139" s="27"/>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
-    </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B140" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="C140" s="39"/>
-      <c r="D140" s="39"/>
-    </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F139" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G139" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H139" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="140" spans="2:8">
+      <c r="B140" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C140" s="37"/>
+      <c r="D140" s="37"/>
+    </row>
+    <row r="141" spans="2:8">
       <c r="B141" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E141" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F141" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F141" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G141" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H141" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="2:8">
       <c r="B142" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C142" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D142" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="D142" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="E142" s="7"/>
-      <c r="F142" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G142" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H142" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B143" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C143" s="39"/>
-      <c r="D143" s="39"/>
-    </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B144" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C144" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D144" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E144" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F144" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B145" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C145" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D145" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E145" s="7"/>
-      <c r="F145" s="8"/>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B146" s="7" t="s">
+      <c r="F142" s="8"/>
+    </row>
+    <row r="143" spans="2:8">
+      <c r="B143" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C146" s="7" t="s">
+      <c r="C143" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D146" s="7"/>
-      <c r="E146" s="7"/>
-      <c r="F146" s="8"/>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B147" s="14" t="s">
+      <c r="D143" s="7"/>
+      <c r="E143" s="7"/>
+      <c r="F143" s="8"/>
+    </row>
+    <row r="144" spans="2:8">
+      <c r="B144" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C147" s="7">
+      <c r="C144" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B148" s="14" t="s">
+    <row r="145" spans="2:3">
+      <c r="B145" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C148" s="7">
+      <c r="C145" s="7">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="25">
+  <mergeCells count="23">
+    <mergeCell ref="B137:D137"/>
     <mergeCell ref="B140:D140"/>
-    <mergeCell ref="B143:D143"/>
     <mergeCell ref="B85:D85"/>
     <mergeCell ref="B88:D88"/>
     <mergeCell ref="B99:E99"/>
     <mergeCell ref="B108:D108"/>
     <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B131:E131"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B128:E128"/>
     <mergeCell ref="B120:D120"/>
-    <mergeCell ref="B125:D125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B122:D122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B135:C135"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="H14:I14"/>
@@ -2565,76 +2521,76 @@
     <brk id="33" max="16383" man="1"/>
     <brk id="73" max="16383" man="1"/>
     <brk id="96" max="16383" man="1"/>
-    <brk id="128" max="16383" man="1"/>
+    <brk id="125" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B58"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="28" customWidth="1"/>
     <col min="2" max="2" width="106.42578125" customWidth="1"/>
     <col min="3" max="3" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="B1" s="29" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
         <v>&lt;forecast seriesName="Influenza"&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="B2" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202"/&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="B3" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Nasal" vaccineIds="180, 203"/&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="B4" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Live" vaccineIds="158, 159, 160, 161, 162, 171, 175, 178, 2020"/&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="B5" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B8&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C8&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="H1N1" vaccineIds="186, 187, 188, 189"/&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="B6" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B9&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C9&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Season Start" vaccineIds="-503"/&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="B7" s="29" t="str">
         <f>"  &lt;seasonal due="&amp;CHAR(34)&amp;Schedules!I17&amp;CHAR(34)&amp;" overdue="&amp;CHAR(34)&amp;Schedules!I18&amp;CHAR(34)&amp;" end="&amp;CHAR(34)&amp;Schedules!I16&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;seasonal due="1 month" overdue="5 months" end="6 months"/&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="B8" s="29" t="str">
         <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B32&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C32&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D32&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;transition name="" age="" vaccineId=""/&gt;</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="30" t="str">
         <f>Schedules!B75</f>
         <v>P1</v>
@@ -2644,91 +2600,91 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="season"&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="B10" s="29" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="B11" s="32" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C78&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D78&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E78&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="B12" s="32" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C79&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D79&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E79&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="B13" s="32" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="B14" s="32" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="B15" s="32" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="B16" s="32" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="B17" s="32" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="B18" s="32" t="str">
         <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B87&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C87&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D87&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E87&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F87&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G87&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H87&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="B19" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B90&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C90&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F90&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="B20" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B91&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C91&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D91&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F91&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E91&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="B21" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B92&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F92&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="H1N1" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="B22" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B93&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F93&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Season Start" schedule="S1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="B23" s="32" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="30" t="str">
         <f>Schedules!B98</f>
         <v>S1</v>
@@ -2738,213 +2694,195 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="S1" dose="1" indication="" label="current season"&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="B25" s="32" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C115&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="3"/&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="B26" s="32" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D101&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E101&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="B27" s="32" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C102&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D102&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E102&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="B28" s="32" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="B29" s="32" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="B30" s="32" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C105&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="B31" s="32" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="B32" s="32" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2">
       <c r="B33" s="32" t="str">
         <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B110&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C110&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D110&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E110&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F110&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G110&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H110&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2">
       <c r="B34" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B113&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C113&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D113&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F113&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E113&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2">
       <c r="B35" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B114&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C114&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D114&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F114&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E114&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="DL FLU 2014" age="" reason="" seasonCompleted="Yes"/&gt;</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="DL FLU 2015" age="" reason="" seasonCompleted="Yes"/&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="B36" s="32" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="A37" s="30" t="str">
         <f>Schedules!B119</f>
-        <v>DL FLU 2014</v>
+        <v>DL FLU 2015</v>
       </c>
       <c r="B37" s="31" t="str">
         <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B119&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;decisionLogic name="DL FLU 2014"&gt;</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">  &lt;decisionLogic name="DL FLU 2015"&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="B38" s="32" t="str">
         <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B121&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D121&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;constant name="Season 2013 Start" value="07/01/2013"/&gt;</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Flu"/&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="B39" s="32" t="str">
-        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B122&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D122&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;constant name="Season 2010 Start" value="07/01/2010"/&gt;</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B123&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D123&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;transition name="Second Dose Needed" value="S2"/&gt;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="B40" s="32" t="str">
-        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B123&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D123&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Flu"/&gt;</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="32" t="str">
-        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B124&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D124&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;constant name="Valid H1N1 Vaccine" value="H1N1"/&gt;</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B126&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;transition name="Second Dose Needed" value="S2"/&gt;</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B127&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B124&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D124&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="No More Doses Needed" value="COMPLETE"/&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="30" t="str">
-        <f>Schedules!B130</f>
+    <row r="41" spans="1:2">
+      <c r="B41" s="32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="30" t="str">
+        <f>Schedules!B127</f>
         <v>S2</v>
       </c>
-      <c r="B45" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B130&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C130&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D130&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E129&amp;CHAR(34)&amp;"&gt;"</f>
+      <c r="B42" s="31" t="str">
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B127&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C127&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E126&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S2" dose="2" indication="" label="2nd seasonal"&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C148&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C147&amp;CHAR(34)&amp;"/&gt;"</f>
+    <row r="43" spans="1:2">
+      <c r="B43" s="29" t="str">
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
+      <c r="B44" s="32" t="str">
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C130&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D130&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E130&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace=""/&gt;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="B45" s="32" t="str">
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C131&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D131&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E131&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" s="32" t="str">
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E132&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;due age="" interval="1 month" grace=""/&gt;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="B47" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace=""/&gt;</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="B48" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
       <c r="B49" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;due age="" interval="1 month" grace=""/&gt;</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
       <c r="B50" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
       <c r="B51" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C137&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E138&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D139&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B139&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C139&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D139&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E139&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F139&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G139&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H139&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="33" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B142&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C142&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D142&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F142&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H142&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E142&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" minInterval="" seasonCompleted=""/&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="33" t="str">
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B143&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C143&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D143&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F143&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H143&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E143&amp;CHAR(34)&amp;"/&gt;"</f>
+        <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="COMPLETE" age="" reason="" minInterval="" seasonCompleted=""/&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
       <c r="B54" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B142&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C142&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D142&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E142&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F142&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G142&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H142&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B145&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D145&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F145&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H145&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E145&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" minInterval="" seasonCompleted=""/&gt;</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B146&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C146&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D146&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F146&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H146&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E146&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="COMPLETE" age="" reason="" minInterval="" seasonCompleted=""/&gt;</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" s="32" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" s="29" t="str">
+    <row r="55" spans="2:2">
+      <c r="B55" s="29" t="str">
         <f>"&lt;/forecast&gt;"</f>
         <v>&lt;/forecast&gt;</v>
       </c>

</xml_diff>

<commit_message>
Added check for invalid dose to Flu2015 logic
</commit_message>
<xml_diff>
--- a/schedules/Influenza.xlsx
+++ b/schedules/Influenza.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="86">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>DL FLU 2015</t>
+  </si>
+  <si>
+    <t>Influenza LAIV4 Nasal</t>
   </si>
 </sst>
 </file>
@@ -1169,8 +1172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IT145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1511,13 +1514,17 @@
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="2:9">
-      <c r="B27" s="19"/>
+      <c r="B27" s="19" t="s">
+        <v>85</v>
+      </c>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
       <c r="E27" s="7">
         <v>203</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="7">
+        <v>149</v>
+      </c>
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="2:9">
@@ -2532,7 +2539,7 @@
   <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1:B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Add support for new Influenza vaccines 168 and 171.
</commit_message>
<xml_diff>
--- a/schedules/Influenza.xlsx
+++ b/schedules/Influenza.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="14085" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358"/>
+    <workbookView xWindow="14085" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$144</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$96</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$96</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$146</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$98</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$98</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="89">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -271,13 +271,22 @@
     <t>Influenza, seasonal, intradermal, preservative free</t>
   </si>
   <si>
-    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202</t>
-  </si>
-  <si>
     <t>DL FLU 2015</t>
   </si>
   <si>
     <t>Influenza LAIV4 Nasal</t>
+  </si>
+  <si>
+    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 218, 219</t>
+  </si>
+  <si>
+    <t>FLUAD, adjuvanted, trivalent, preservative free</t>
+  </si>
+  <si>
+    <t>Flucelvax, injectable, quadrivalent, preservative free</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -634,12 +643,19 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -670,13 +686,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,13 +777,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>346717</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>582084</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>121627</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -788,7 +797,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -808,7 +817,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1103,7 +1112,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1145,7 +1154,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1162,7 +1171,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1170,10 +1179,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IT145"/>
+  <dimension ref="A1:IT147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -1214,83 +1223,83 @@
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
+      <c r="C4" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B5" s="47"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="45"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="2:9" ht="12.75" customHeight="1">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="40">
         <v>-503</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="11" t="s">
@@ -1329,10 +1338,10 @@
       <c r="F14" s="7">
         <v>111</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="37"/>
+      <c r="I14" s="36"/>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="19" t="s">
@@ -1515,7 +1524,7 @@
     </row>
     <row r="27" spans="2:9">
       <c r="B27" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
@@ -1542,12 +1551,37 @@
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="2:9">
+      <c r="B29" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="7">
+        <v>218</v>
+      </c>
+      <c r="F29" s="7">
+        <v>168</v>
+      </c>
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="2:9">
+      <c r="B30" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="7">
+        <v>219</v>
+      </c>
+      <c r="F30" s="7">
+        <v>171</v>
+      </c>
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="2:9">
+      <c r="E31" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="I31" s="9"/>
     </row>
     <row r="32" spans="2:9">
@@ -1677,116 +1711,94 @@
       <c r="I73" s="9"/>
     </row>
     <row r="74" spans="2:11">
-      <c r="B74" s="10" t="s">
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="2:11">
+      <c r="I75" s="9"/>
+    </row>
+    <row r="76" spans="2:11">
+      <c r="B76" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C76" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D74" s="10" t="s">
+      <c r="D76" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E74" s="22" t="s">
+      <c r="E76" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="I74" s="9"/>
-    </row>
-    <row r="75" spans="2:11">
-      <c r="B75" s="23" t="s">
+      <c r="I76" s="9"/>
+    </row>
+    <row r="77" spans="2:11">
+      <c r="B77" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C75" s="23">
+      <c r="C77" s="23">
         <v>1</v>
       </c>
-      <c r="D75" s="23" t="s">
+      <c r="D77" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="I75" s="9"/>
-    </row>
-    <row r="76" spans="2:11">
-      <c r="B76" s="37" t="s">
+      <c r="I77" s="9"/>
+    </row>
+    <row r="78" spans="2:11">
+      <c r="B78" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="I76" s="9"/>
-    </row>
-    <row r="77" spans="2:11">
-      <c r="B77" s="24"/>
-      <c r="C77" s="5" t="s">
+      <c r="C78" s="36"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="36"/>
+      <c r="I78" s="9"/>
+    </row>
+    <row r="79" spans="2:11">
+      <c r="B79" s="24"/>
+      <c r="C79" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D79" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E77" s="5" t="s">
+      <c r="E79" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I77" s="9"/>
-    </row>
-    <row r="78" spans="2:11">
-      <c r="B78" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9"/>
-      <c r="K78" s="25"/>
-    </row>
-    <row r="79" spans="2:11">
-      <c r="B79" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
       <c r="I79" s="9"/>
-      <c r="J79" s="9"/>
-      <c r="K79" s="25"/>
     </row>
     <row r="80" spans="2:11">
       <c r="B80" s="14" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D80" s="7"/>
-      <c r="E80" s="7"/>
-      <c r="H80" s="25"/>
+      <c r="D80" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="I80" s="9"/>
       <c r="J80" s="9"/>
       <c r="K80" s="25"/>
     </row>
     <row r="81" spans="2:11">
       <c r="B81" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
-      <c r="H81" s="25"/>
       <c r="I81" s="9"/>
       <c r="J81" s="9"/>
       <c r="K81" s="25"/>
     </row>
     <row r="82" spans="2:11">
       <c r="B82" s="14" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
@@ -1796,13 +1808,13 @@
       <c r="K82" s="25"/>
     </row>
     <row r="83" spans="2:11">
-      <c r="B83" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C83" s="27"/>
-      <c r="D83" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="B83" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="H83" s="25"/>
       <c r="I83" s="9"/>
@@ -1810,10 +1822,12 @@
       <c r="K83" s="25"/>
     </row>
     <row r="84" spans="2:11">
-      <c r="B84" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C84" s="27"/>
+      <c r="B84" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
       <c r="H84" s="25"/>
@@ -1822,136 +1836,136 @@
       <c r="K84" s="25"/>
     </row>
     <row r="85" spans="2:11">
-      <c r="B85" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C85" s="37"/>
-      <c r="D85" s="37"/>
+      <c r="B85" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C85" s="27"/>
+      <c r="D85" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E85" s="7"/>
       <c r="H85" s="25"/>
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
       <c r="K85" s="25"/>
     </row>
     <row r="86" spans="2:11">
-      <c r="B86" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G86" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H86" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="B86" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C86" s="27"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="H86" s="25"/>
       <c r="I86" s="9"/>
       <c r="J86" s="9"/>
       <c r="K86" s="25"/>
     </row>
     <row r="87" spans="2:11">
-      <c r="B87" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D87" s="7"/>
-      <c r="E87" s="7"/>
-      <c r="F87" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G87" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="B87" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C87" s="36"/>
+      <c r="D87" s="36"/>
+      <c r="H87" s="25"/>
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
+      <c r="K87" s="25"/>
     </row>
     <row r="88" spans="2:11">
-      <c r="B88" s="37" t="s">
+      <c r="B88" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I88" s="9"/>
+      <c r="J88" s="9"/>
+      <c r="K88" s="25"/>
+    </row>
+    <row r="89" spans="2:11">
+      <c r="B89" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+    </row>
+    <row r="90" spans="2:11">
+      <c r="B90" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C88" s="37"/>
-      <c r="D88" s="37"/>
-      <c r="J88" s="9"/>
-    </row>
-    <row r="89" spans="2:11">
-      <c r="B89" s="5" t="s">
+      <c r="C90" s="36"/>
+      <c r="D90" s="36"/>
+      <c r="J90" s="9"/>
+    </row>
+    <row r="91" spans="2:11">
+      <c r="B91" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C89" s="5" t="s">
+      <c r="C91" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D91" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E89" s="5" t="s">
+      <c r="E91" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F89" s="5" t="s">
+      <c r="F91" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J89" s="9"/>
-    </row>
-    <row r="90" spans="2:11">
-      <c r="B90" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E90" s="7"/>
-      <c r="F90" s="8"/>
-      <c r="J90" s="9"/>
-      <c r="K90" s="25"/>
-    </row>
-    <row r="91" spans="2:11">
-      <c r="B91" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="8"/>
       <c r="J91" s="9"/>
-      <c r="K91" s="25"/>
     </row>
     <row r="92" spans="2:11">
       <c r="B92" s="7" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D92" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="E92" s="7"/>
-      <c r="F92" s="35"/>
+      <c r="F92" s="8"/>
       <c r="J92" s="9"/>
       <c r="K92" s="25"/>
     </row>
     <row r="93" spans="2:11">
       <c r="B93" s="7" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
@@ -1960,562 +1974,588 @@
       <c r="K93" s="25"/>
     </row>
     <row r="94" spans="2:11">
-      <c r="B94" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C94" s="7">
-        <v>1</v>
-      </c>
+      <c r="B94" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="35"/>
       <c r="J94" s="9"/>
       <c r="K94" s="25"/>
     </row>
     <row r="95" spans="2:11">
-      <c r="B95" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C95" s="7">
-        <v>1</v>
-      </c>
-      <c r="H95" s="25"/>
-      <c r="I95" s="9"/>
+      <c r="B95" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="8"/>
       <c r="J95" s="9"/>
       <c r="K95" s="25"/>
     </row>
     <row r="96" spans="2:11">
-      <c r="H96" s="25"/>
-      <c r="I96" s="9"/>
+      <c r="B96" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C96" s="7">
+        <v>1</v>
+      </c>
       <c r="J96" s="9"/>
       <c r="K96" s="25"/>
     </row>
-    <row r="97" spans="2:8">
-      <c r="B97" s="10" t="s">
+    <row r="97" spans="2:11">
+      <c r="B97" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C97" s="7">
+        <v>1</v>
+      </c>
+      <c r="H97" s="25"/>
+      <c r="I97" s="9"/>
+      <c r="J97" s="9"/>
+      <c r="K97" s="25"/>
+    </row>
+    <row r="98" spans="2:11">
+      <c r="H98" s="25"/>
+      <c r="I98" s="9"/>
+      <c r="J98" s="9"/>
+      <c r="K98" s="25"/>
+    </row>
+    <row r="99" spans="2:11">
+      <c r="B99" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C99" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D97" s="10" t="s">
+      <c r="D99" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E97" s="22" t="s">
+      <c r="E99" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="F97" s="22"/>
-    </row>
-    <row r="98" spans="2:8">
-      <c r="B98" s="23" t="s">
+      <c r="F99" s="22"/>
+    </row>
+    <row r="100" spans="2:11">
+      <c r="B100" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C98" s="23">
+      <c r="C100" s="23">
         <v>1</v>
       </c>
-      <c r="D98" s="23"/>
-    </row>
-    <row r="99" spans="2:8">
-      <c r="B99" s="37" t="s">
+      <c r="D100" s="23"/>
+    </row>
+    <row r="101" spans="2:11">
+      <c r="B101" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C99" s="37"/>
-      <c r="D99" s="37"/>
-      <c r="E99" s="37"/>
-    </row>
-    <row r="100" spans="2:8">
-      <c r="B100" s="24"/>
-      <c r="C100" s="5" t="s">
+      <c r="C101" s="36"/>
+      <c r="D101" s="36"/>
+      <c r="E101" s="36"/>
+    </row>
+    <row r="102" spans="2:11">
+      <c r="B102" s="24"/>
+      <c r="C102" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D102" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E100" s="5" t="s">
+      <c r="E102" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="2:8">
-      <c r="B101" s="14" t="s">
+    <row r="103" spans="2:11">
+      <c r="B103" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D101" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E101" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="102" spans="2:8">
-      <c r="B102" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
-      <c r="E102" s="7"/>
-    </row>
-    <row r="103" spans="2:8">
-      <c r="B103" s="14" t="s">
-        <v>20</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D103" s="7"/>
-      <c r="E103" s="7"/>
-    </row>
-    <row r="104" spans="2:8">
+      <c r="D103" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="2:11">
       <c r="B104" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="2:8">
+    <row r="105" spans="2:11">
       <c r="B105" s="14" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="2:8">
-      <c r="B106" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C106" s="27"/>
-      <c r="D106" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="107" spans="2:8">
-      <c r="B107" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C107" s="27"/>
+    <row r="106" spans="2:11">
+      <c r="B106" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+    </row>
+    <row r="107" spans="2:11">
+      <c r="B107" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="2:8">
-      <c r="B108" s="37" t="s">
+    <row r="108" spans="2:11">
+      <c r="B108" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C108" s="27"/>
+      <c r="D108" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="109" spans="2:11">
+      <c r="B109" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C109" s="27"/>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+    </row>
+    <row r="110" spans="2:11">
+      <c r="B110" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C108" s="37"/>
-      <c r="D108" s="37"/>
-    </row>
-    <row r="109" spans="2:8">
-      <c r="B109" s="5" t="s">
+      <c r="C110" s="36"/>
+      <c r="D110" s="36"/>
+    </row>
+    <row r="111" spans="2:11">
+      <c r="B111" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="C111" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="D111" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E109" s="5" t="s">
+      <c r="E111" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F109" s="5" t="s">
+      <c r="F111" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G109" s="5" t="s">
+      <c r="G111" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H109" s="5" t="s">
+      <c r="H111" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="110" spans="2:8">
-      <c r="B110" s="7" t="s">
+    <row r="112" spans="2:11">
+      <c r="B112" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C110" s="7" t="s">
+      <c r="C112" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D110" s="7"/>
-      <c r="E110" s="7"/>
-      <c r="F110" s="7" t="s">
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G110" s="7" t="s">
+      <c r="G112" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H110" s="7" t="s">
+      <c r="H112" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="2:8">
-      <c r="B111" s="37" t="s">
+    <row r="113" spans="2:6">
+      <c r="B113" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C111" s="37"/>
-      <c r="D111" s="37"/>
-    </row>
-    <row r="112" spans="2:8">
-      <c r="B112" s="5" t="s">
+      <c r="C113" s="36"/>
+      <c r="D113" s="36"/>
+    </row>
+    <row r="114" spans="2:6">
+      <c r="B114" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C112" s="5" t="s">
+      <c r="C114" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="D114" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E112" s="5" t="s">
+      <c r="E114" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F112" s="5" t="s">
+      <c r="F114" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="113" spans="2:6">
-      <c r="B113" s="7" t="s">
+    <row r="115" spans="2:6">
+      <c r="B115" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C113" s="7" t="s">
+      <c r="C115" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D113" s="7" t="s">
+      <c r="D115" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E113" s="7"/>
-      <c r="F113" s="8"/>
-    </row>
-    <row r="114" spans="2:6">
-      <c r="B114" s="7" t="s">
+      <c r="E115" s="7"/>
+      <c r="F115" s="8"/>
+    </row>
+    <row r="116" spans="2:6">
+      <c r="B116" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C114" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D114" s="7"/>
-      <c r="E114" s="7" t="s">
+      <c r="C116" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D116" s="7"/>
+      <c r="E116" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F114" s="8"/>
-    </row>
-    <row r="115" spans="2:6">
-      <c r="B115" s="14" t="s">
+      <c r="F116" s="8"/>
+    </row>
+    <row r="117" spans="2:6">
+      <c r="B117" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C115" s="7">
+      <c r="C117" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="2:6">
-      <c r="B116" s="14" t="s">
+    <row r="118" spans="2:6">
+      <c r="B118" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C116" s="7">
+      <c r="C118" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="2:6">
-      <c r="B118" s="10" t="s">
+    <row r="120" spans="2:6">
+      <c r="B120" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="119" spans="2:6">
-      <c r="B119" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6">
-      <c r="B120" s="37" t="s">
+    <row r="121" spans="2:6">
+      <c r="B121" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6">
+      <c r="B122" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C120" s="37"/>
-      <c r="D120" s="37"/>
-    </row>
-    <row r="121" spans="2:6">
-      <c r="B121" s="11" t="s">
+      <c r="C122" s="36"/>
+      <c r="D122" s="36"/>
+    </row>
+    <row r="123" spans="2:6">
+      <c r="B123" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C121" s="13"/>
-      <c r="D121" s="34" t="s">
+      <c r="C123" s="13"/>
+      <c r="D123" s="34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="2:6">
-      <c r="B122" s="37" t="s">
+    <row r="124" spans="2:6">
+      <c r="B124" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C122" s="37"/>
-      <c r="D122" s="37"/>
-    </row>
-    <row r="123" spans="2:6">
-      <c r="B123" s="48" t="s">
+      <c r="C124" s="36"/>
+      <c r="D124" s="36"/>
+    </row>
+    <row r="125" spans="2:6">
+      <c r="B125" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="C123" s="49"/>
-      <c r="D123" s="34" t="s">
+      <c r="C125" s="38"/>
+      <c r="D125" s="34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="124" spans="2:6">
-      <c r="B124" s="48" t="s">
+    <row r="126" spans="2:6">
+      <c r="B126" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="C124" s="49"/>
-      <c r="D124" s="34" t="s">
+      <c r="C126" s="38"/>
+      <c r="D126" s="34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="126" spans="2:6">
-      <c r="B126" s="10" t="s">
+    <row r="128" spans="2:6">
+      <c r="B128" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C126" s="10" t="s">
+      <c r="C128" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E126" s="22" t="s">
+      <c r="E128" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F126" s="22"/>
-    </row>
-    <row r="127" spans="2:6">
-      <c r="B127" s="23" t="s">
+      <c r="F128" s="22"/>
+    </row>
+    <row r="129" spans="2:8">
+      <c r="B129" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C127" s="23">
+      <c r="C129" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="128" spans="2:6">
-      <c r="B128" s="37" t="s">
+    <row r="130" spans="2:8">
+      <c r="B130" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C128" s="37"/>
-      <c r="D128" s="37"/>
-      <c r="E128" s="37"/>
-    </row>
-    <row r="129" spans="2:8">
-      <c r="B129" s="24"/>
-      <c r="C129" s="5" t="s">
+      <c r="C130" s="36"/>
+      <c r="D130" s="36"/>
+      <c r="E130" s="36"/>
+    </row>
+    <row r="131" spans="2:8">
+      <c r="B131" s="24"/>
+      <c r="C131" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D129" s="5" t="s">
+      <c r="D131" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E129" s="5" t="s">
+      <c r="E131" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="130" spans="2:8">
-      <c r="B130" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C130" s="7"/>
-      <c r="D130" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E130" s="7"/>
-    </row>
-    <row r="131" spans="2:8">
-      <c r="B131" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C131" s="7"/>
-      <c r="D131" s="7"/>
-      <c r="E131" s="7"/>
     </row>
     <row r="132" spans="2:8">
       <c r="B132" s="14" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C132" s="7"/>
       <c r="D132" s="7" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E132" s="7"/>
     </row>
     <row r="133" spans="2:8">
       <c r="B133" s="14" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C133" s="7"/>
-      <c r="D133" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="D133" s="7"/>
       <c r="E133" s="7"/>
     </row>
     <row r="134" spans="2:8">
       <c r="B134" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C134" s="7"/>
+      <c r="D134" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E134" s="7"/>
+    </row>
+    <row r="135" spans="2:8">
+      <c r="B135" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C135" s="7"/>
+      <c r="D135" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E135" s="7"/>
+    </row>
+    <row r="136" spans="2:8">
+      <c r="B136" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C134" s="7" t="s">
+      <c r="C136" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D134" s="7"/>
-      <c r="E134" s="7"/>
-    </row>
-    <row r="135" spans="2:8">
-      <c r="B135" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="C135" s="50"/>
-      <c r="D135" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E135" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="136" spans="2:8">
-      <c r="B136" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C136" s="27"/>
       <c r="D136" s="7"/>
       <c r="E136" s="7"/>
     </row>
     <row r="137" spans="2:8">
-      <c r="B137" s="37" t="s">
+      <c r="B137" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C137" s="39"/>
+      <c r="D137" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E137" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8">
+      <c r="B138" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C138" s="27"/>
+      <c r="D138" s="7"/>
+      <c r="E138" s="7"/>
+    </row>
+    <row r="139" spans="2:8">
+      <c r="B139" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C137" s="37"/>
-      <c r="D137" s="37"/>
-    </row>
-    <row r="138" spans="2:8">
-      <c r="B138" s="5" t="s">
+      <c r="C139" s="36"/>
+      <c r="D139" s="36"/>
+    </row>
+    <row r="140" spans="2:8">
+      <c r="B140" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C138" s="5" t="s">
+      <c r="C140" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D138" s="5" t="s">
+      <c r="D140" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E138" s="5" t="s">
+      <c r="E140" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F138" s="5" t="s">
+      <c r="F140" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G138" s="5" t="s">
+      <c r="G140" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H138" s="5" t="s">
+      <c r="H140" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="139" spans="2:8">
-      <c r="B139" s="7" t="s">
+    <row r="141" spans="2:8">
+      <c r="B141" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C139" s="7" t="s">
+      <c r="C141" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D139" s="7"/>
-      <c r="E139" s="7"/>
-      <c r="F139" s="7" t="s">
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
+      <c r="F141" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G139" s="7" t="s">
+      <c r="G141" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H139" s="7" t="s">
+      <c r="H141" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="140" spans="2:8">
-      <c r="B140" s="37" t="s">
+    <row r="142" spans="2:8">
+      <c r="B142" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C140" s="37"/>
-      <c r="D140" s="37"/>
-    </row>
-    <row r="141" spans="2:8">
-      <c r="B141" s="5" t="s">
+      <c r="C142" s="36"/>
+      <c r="D142" s="36"/>
+    </row>
+    <row r="143" spans="2:8">
+      <c r="B143" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C141" s="5" t="s">
+      <c r="C143" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D141" s="5" t="s">
+      <c r="D143" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E141" s="5" t="s">
+      <c r="E143" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F141" s="5" t="s">
+      <c r="F143" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="142" spans="2:8">
-      <c r="B142" s="7" t="s">
+    <row r="144" spans="2:8">
+      <c r="B144" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C142" s="7" t="s">
+      <c r="C144" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D142" s="7" t="s">
+      <c r="D144" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E142" s="7"/>
-      <c r="F142" s="8"/>
-    </row>
-    <row r="143" spans="2:8">
-      <c r="B143" s="7" t="s">
+      <c r="E144" s="7"/>
+      <c r="F144" s="8"/>
+    </row>
+    <row r="145" spans="2:6">
+      <c r="B145" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C143" s="7" t="s">
+      <c r="C145" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D143" s="7"/>
-      <c r="E143" s="7"/>
-      <c r="F143" s="8"/>
-    </row>
-    <row r="144" spans="2:8">
-      <c r="B144" s="14" t="s">
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="8"/>
+    </row>
+    <row r="146" spans="2:6">
+      <c r="B146" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C144" s="7">
+      <c r="C146" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="2:3">
-      <c r="B145" s="14" t="s">
+    <row r="147" spans="2:6">
+      <c r="B147" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C145" s="7">
+      <c r="C147" s="7">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="23">
-    <mergeCell ref="B137:D137"/>
-    <mergeCell ref="B140:D140"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B99:E99"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B128:E128"/>
-    <mergeCell ref="B120:D120"/>
-    <mergeCell ref="B122:D122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B135:C135"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="B78:E78"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C4:F5"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B139:D139"/>
+    <mergeCell ref="B142:D142"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B101:E101"/>
+    <mergeCell ref="B110:D110"/>
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="B130:E130"/>
+    <mergeCell ref="B122:D122"/>
+    <mergeCell ref="B124:D124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B137:C137"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2525,10 +2565,10 @@
     <oddFooter>&amp;CPrepared by  Nathan Bunker &amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <rowBreaks count="4" manualBreakCount="4">
-    <brk id="33" max="16383" man="1"/>
-    <brk id="73" max="16383" man="1"/>
-    <brk id="96" max="16383" man="1"/>
-    <brk id="125" max="16383" man="1"/>
+    <brk id="35" max="16383" man="1"/>
+    <brk id="75" max="16383" man="1"/>
+    <brk id="98" max="16383" man="1"/>
+    <brk id="127" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -2538,8 +2578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B55"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -2558,7 +2598,7 @@
     <row r="2" spans="1:2">
       <c r="B2" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 218, 219"/&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2593,95 +2633,95 @@
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="29" t="str">
-        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B32&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C32&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D32&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B34&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C34&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;transition name="" age="" vaccineId=""/&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="30" t="str">
-        <f>Schedules!B75</f>
+        <f>Schedules!B77</f>
         <v>P1</v>
       </c>
       <c r="B9" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B75&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C75&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D75&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E74&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B77&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C77&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D77&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E76&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="season"&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="B10" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="B11" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C78&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D78&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E78&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="B12" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C79&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D79&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E79&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="B13" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="B14" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="B15" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="B16" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="B17" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="B18" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B87&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C87&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D87&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E87&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F87&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G87&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H87&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B89&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C89&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E89&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F89&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G89&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H89&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="B19" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B90&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C90&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F90&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B92&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F92&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="B20" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B91&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C91&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D91&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F91&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E91&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B93&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F93&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="B21" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B92&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F92&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B94&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F94&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E94&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="H1N1" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="B22" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B93&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F93&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B95&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F95&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Season Start" schedule="S1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
@@ -2693,77 +2733,77 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="30" t="str">
-        <f>Schedules!B98</f>
+        <f>Schedules!B100</f>
         <v>S1</v>
       </c>
       <c r="B24" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B98&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D98&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E97&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B100&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D100&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E99&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S1" dose="1" indication="" label="current season"&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="B25" s="32" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C115&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C117&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="3"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="B26" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D101&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E101&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="B27" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C102&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D102&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E102&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="B28" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C105&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="B29" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="B30" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C105&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="B31" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="B32" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="B33" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B110&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C110&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D110&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E110&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F110&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G110&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H110&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B112&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C112&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E112&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F112&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G112&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H112&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="B34" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B113&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C113&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D113&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F113&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E113&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B115&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C115&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D115&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F115&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E115&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="B35" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B114&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C114&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D114&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F114&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E114&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B116&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D116&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F116&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E116&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="DL FLU 2015" age="" reason="" seasonCompleted="Yes"/&gt;</v>
       </c>
     </row>
@@ -2775,29 +2815,29 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="30" t="str">
-        <f>Schedules!B119</f>
+        <f>Schedules!B121</f>
         <v>DL FLU 2015</v>
       </c>
       <c r="B37" s="31" t="str">
-        <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B119&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B121&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;decisionLogic name="DL FLU 2015"&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="B38" s="32" t="str">
-        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B121&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D121&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B123&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D123&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Flu"/&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="B39" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B123&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D123&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B125&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D125&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Second Dose Needed" value="S2"/&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="B40" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B124&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D124&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B126&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="No More Doses Needed" value="COMPLETE"/&gt;</v>
       </c>
     </row>
@@ -2808,77 +2848,77 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="30" t="str">
-        <f>Schedules!B127</f>
+        <f>Schedules!B129</f>
         <v>S2</v>
       </c>
       <c r="B42" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B127&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C127&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E126&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B129&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C129&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D129&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E128&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S2" dose="2" indication="" label="2nd seasonal"&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="B43" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C147&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C146&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="B44" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C130&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D130&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E130&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E132&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="B45" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C131&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D131&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E131&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="B46" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E132&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="1 month" grace=""/&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="B47" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="B48" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B139&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C139&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D139&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E139&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F139&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G139&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H139&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B141&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C141&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D141&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E141&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F141&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G141&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H141&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B142&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C142&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D142&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F142&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H142&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E142&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B144&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F144&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H144&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E144&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B143&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C143&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D143&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F143&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H143&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E143&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B145&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D145&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F145&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H145&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E145&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="COMPLETE" age="" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add vaccine ID's to the schedule for the following vaccines: - CVX 166 - TCH 217: influenza, intradermal, quadrivalent, preservative free - CVX 151 - TCH 220: Influenza nasal, unspecified formulation
- CVX 185 - TCH 221: influenza recombinant quadrivalent 
- CVX 186 - TCH 222: Influenza injectable MDCK quadrivalent
</commit_message>
<xml_diff>
--- a/schedules/Influenza.xlsx
+++ b/schedules/Influenza.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCHWorkspaceJava6\fv\schedules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14085" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358" activeTab="1"/>
+    <workbookView xWindow="15390" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
@@ -15,12 +20,12 @@
     <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$98</definedName>
     <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$98</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="92">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -277,23 +282,32 @@
     <t>Influenza LAIV4 Nasal</t>
   </si>
   <si>
-    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 218, 219</t>
-  </si>
-  <si>
     <t>FLUAD, adjuvanted, trivalent, preservative free</t>
   </si>
   <si>
     <t>Flucelvax, injectable, quadrivalent, preservative free</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 217, 218, 219, 220, 221, 222</t>
+  </si>
+  <si>
+    <t>influenza, intradermal, quadrivalent, preservative free</t>
+  </si>
+  <si>
+    <t>influenza nasal, unspecified formulation</t>
+  </si>
+  <si>
+    <t>influenza recombinant quadrivalent</t>
+  </si>
+  <si>
+    <t>influenza injectable MDCK quadrivalent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -643,9 +657,42 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -653,39 +700,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,7 +811,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -817,7 +831,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1112,7 +1126,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1154,7 +1168,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1171,21 +1185,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IT147"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
     <col min="2" max="5" width="14.28515625" style="1" customWidth="1"/>
@@ -1209,8 +1223,8 @@
     <col min="23" max="254" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="8.25" customHeight="1"/>
-    <row r="2" spans="2:9">
+    <row r="1" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1219,89 +1233,89 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-    </row>
-    <row r="4" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B4" s="49" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+    </row>
+    <row r="4" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="45"/>
-    </row>
-    <row r="5" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B5" s="50"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
-    </row>
-    <row r="6" spans="2:9" ht="12.75" customHeight="1">
+      <c r="C4" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
+    </row>
+    <row r="5" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="47"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="45"/>
+    </row>
+    <row r="6" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-    </row>
-    <row r="7" spans="2:9">
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-    </row>
-    <row r="8" spans="2:9">
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-    </row>
-    <row r="9" spans="2:9">
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="36">
         <v>-503</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="36" t="s">
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-    </row>
-    <row r="12" spans="2:9">
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
@@ -1326,7 +1340,7 @@
       <c r="F13" s="7"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>17</v>
       </c>
@@ -1338,12 +1352,12 @@
       <c r="F14" s="7">
         <v>111</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="36"/>
-    </row>
-    <row r="15" spans="2:9">
+      <c r="I14" s="37"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>19</v>
       </c>
@@ -1362,7 +1376,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
@@ -1379,7 +1393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="15" t="s">
         <v>22</v>
       </c>
@@ -1396,7 +1410,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
         <v>1</v>
       </c>
@@ -1415,7 +1429,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
         <v>23</v>
       </c>
@@ -1428,7 +1442,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
         <v>24</v>
       </c>
@@ -1442,7 +1456,7 @@
       </c>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
         <v>25</v>
       </c>
@@ -1456,7 +1470,7 @@
       </c>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
         <v>26</v>
       </c>
@@ -1470,7 +1484,7 @@
       </c>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
         <v>27</v>
       </c>
@@ -1484,7 +1498,7 @@
       </c>
       <c r="I23" s="9"/>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="19" t="s">
         <v>28</v>
       </c>
@@ -1498,7 +1512,7 @@
       </c>
       <c r="I24" s="9"/>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="19" t="s">
         <v>29</v>
       </c>
@@ -1512,7 +1526,7 @@
       </c>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="19"/>
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
@@ -1522,7 +1536,7 @@
       <c r="F26" s="7"/>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="19" t="s">
         <v>84</v>
       </c>
@@ -1536,7 +1550,7 @@
       </c>
       <c r="I27" s="9"/>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="19" t="s">
         <v>82</v>
       </c>
@@ -1550,173 +1564,214 @@
       </c>
       <c r="I28" s="9"/>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="21"/>
       <c r="E29" s="7">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F29" s="7">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="21"/>
       <c r="E30" s="7">
+        <v>218</v>
+      </c>
+      <c r="F30" s="7">
+        <v>168</v>
+      </c>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="7">
         <v>219</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F31" s="7">
         <v>171</v>
       </c>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="2:9">
-      <c r="E31" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="I31" s="9"/>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="7">
+        <v>220</v>
+      </c>
+      <c r="F32" s="7">
+        <v>151</v>
+      </c>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="9:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="7">
+        <v>221</v>
+      </c>
+      <c r="F33" s="7">
+        <v>185</v>
+      </c>
       <c r="I33" s="9"/>
     </row>
-    <row r="34" spans="9:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="7">
+        <v>222</v>
+      </c>
+      <c r="F34" s="7">
+        <v>186</v>
+      </c>
       <c r="I34" s="9"/>
     </row>
-    <row r="35" spans="9:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I35" s="9"/>
     </row>
-    <row r="36" spans="9:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I36" s="9"/>
     </row>
-    <row r="37" spans="9:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I37" s="9"/>
     </row>
-    <row r="38" spans="9:9">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I38" s="9"/>
     </row>
-    <row r="39" spans="9:9">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="9:9">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I40" s="9"/>
     </row>
-    <row r="41" spans="9:9">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I41" s="9"/>
     </row>
-    <row r="42" spans="9:9">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I42" s="9"/>
     </row>
-    <row r="43" spans="9:9">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I43" s="9"/>
     </row>
-    <row r="44" spans="9:9">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I44" s="9"/>
     </row>
-    <row r="45" spans="9:9">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I45" s="9"/>
     </row>
-    <row r="46" spans="9:9">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I46" s="9"/>
     </row>
-    <row r="47" spans="9:9">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I47" s="9"/>
     </row>
-    <row r="48" spans="9:9">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I48" s="9"/>
     </row>
-    <row r="49" spans="9:9">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I49" s="9"/>
     </row>
-    <row r="50" spans="9:9">
+    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I50" s="9"/>
     </row>
-    <row r="51" spans="9:9">
+    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I51" s="9"/>
     </row>
-    <row r="52" spans="9:9">
+    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I52" s="9"/>
     </row>
-    <row r="53" spans="9:9">
+    <row r="53" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I53" s="9"/>
     </row>
-    <row r="54" spans="9:9">
+    <row r="54" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I54" s="9"/>
     </row>
-    <row r="55" spans="9:9">
+    <row r="55" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I55" s="9"/>
     </row>
-    <row r="56" spans="9:9">
+    <row r="56" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I56" s="9"/>
     </row>
-    <row r="57" spans="9:9">
+    <row r="57" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I57" s="9"/>
     </row>
-    <row r="58" spans="9:9">
+    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I58" s="9"/>
     </row>
-    <row r="59" spans="9:9">
+    <row r="59" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I59" s="9"/>
     </row>
-    <row r="60" spans="9:9">
+    <row r="60" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I60" s="9"/>
     </row>
-    <row r="61" spans="9:9">
+    <row r="61" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I61" s="9"/>
     </row>
-    <row r="62" spans="9:9">
+    <row r="62" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I62" s="9"/>
     </row>
-    <row r="63" spans="9:9">
+    <row r="63" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I63" s="9"/>
     </row>
-    <row r="64" spans="9:9">
+    <row r="64" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I64" s="9"/>
     </row>
-    <row r="65" spans="2:11">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I65" s="9"/>
     </row>
-    <row r="66" spans="2:11">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I66" s="9"/>
     </row>
-    <row r="67" spans="2:11">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I67" s="9"/>
     </row>
-    <row r="68" spans="2:11">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I68" s="9"/>
     </row>
-    <row r="69" spans="2:11">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I69" s="9"/>
     </row>
-    <row r="70" spans="2:11">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I70" s="9"/>
     </row>
-    <row r="71" spans="2:11">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I71" s="9"/>
     </row>
-    <row r="72" spans="2:11">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I72" s="9"/>
     </row>
-    <row r="73" spans="2:11">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I73" s="9"/>
     </row>
-    <row r="74" spans="2:11">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I74" s="9"/>
     </row>
-    <row r="75" spans="2:11">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
       <c r="I75" s="9"/>
     </row>
-    <row r="76" spans="2:11">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B76" s="10" t="s">
         <v>32</v>
       </c>
@@ -1731,7 +1786,7 @@
       </c>
       <c r="I76" s="9"/>
     </row>
-    <row r="77" spans="2:11">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B77" s="23" t="s">
         <v>35</v>
       </c>
@@ -1743,16 +1798,16 @@
       </c>
       <c r="I77" s="9"/>
     </row>
-    <row r="78" spans="2:11">
-      <c r="B78" s="36" t="s">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B78" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="37"/>
       <c r="I78" s="9"/>
     </row>
-    <row r="79" spans="2:11">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B79" s="24"/>
       <c r="C79" s="5" t="s">
         <v>31</v>
@@ -1765,7 +1820,7 @@
       </c>
       <c r="I79" s="9"/>
     </row>
-    <row r="80" spans="2:11">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B80" s="14" t="s">
         <v>40</v>
       </c>
@@ -1782,7 +1837,7 @@
       <c r="J80" s="9"/>
       <c r="K80" s="25"/>
     </row>
-    <row r="81" spans="2:11">
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" s="14" t="s">
         <v>42</v>
       </c>
@@ -1793,7 +1848,7 @@
       <c r="J81" s="9"/>
       <c r="K81" s="25"/>
     </row>
-    <row r="82" spans="2:11">
+    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" s="14" t="s">
         <v>20</v>
       </c>
@@ -1807,7 +1862,7 @@
       <c r="J82" s="9"/>
       <c r="K82" s="25"/>
     </row>
-    <row r="83" spans="2:11">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" s="14" t="s">
         <v>21</v>
       </c>
@@ -1821,7 +1876,7 @@
       <c r="J83" s="9"/>
       <c r="K83" s="25"/>
     </row>
-    <row r="84" spans="2:11">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" s="14" t="s">
         <v>44</v>
       </c>
@@ -1835,7 +1890,7 @@
       <c r="J84" s="9"/>
       <c r="K84" s="25"/>
     </row>
-    <row r="85" spans="2:11">
+    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" s="26" t="s">
         <v>45</v>
       </c>
@@ -1849,7 +1904,7 @@
       <c r="J85" s="9"/>
       <c r="K85" s="25"/>
     </row>
-    <row r="86" spans="2:11">
+    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" s="26" t="s">
         <v>47</v>
       </c>
@@ -1861,18 +1916,18 @@
       <c r="J86" s="9"/>
       <c r="K86" s="25"/>
     </row>
-    <row r="87" spans="2:11">
-      <c r="B87" s="36" t="s">
+    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B87" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C87" s="36"/>
-      <c r="D87" s="36"/>
+      <c r="C87" s="37"/>
+      <c r="D87" s="37"/>
       <c r="H87" s="25"/>
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
       <c r="K87" s="25"/>
     </row>
-    <row r="88" spans="2:11">
+    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="5" t="s">
         <v>9</v>
       </c>
@@ -1898,7 +1953,7 @@
       <c r="J88" s="9"/>
       <c r="K88" s="25"/>
     </row>
-    <row r="89" spans="2:11">
+    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B89" s="7" t="s">
         <v>6</v>
       </c>
@@ -1919,15 +1974,15 @@
       <c r="I89" s="9"/>
       <c r="J89" s="9"/>
     </row>
-    <row r="90" spans="2:11">
-      <c r="B90" s="36" t="s">
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B90" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C90" s="36"/>
-      <c r="D90" s="36"/>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
       <c r="J90" s="9"/>
     </row>
-    <row r="91" spans="2:11">
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" s="5" t="s">
         <v>9</v>
       </c>
@@ -1945,7 +2000,7 @@
       </c>
       <c r="J91" s="9"/>
     </row>
-    <row r="92" spans="2:11">
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" s="7" t="s">
         <v>5</v>
       </c>
@@ -1960,7 +2015,7 @@
       <c r="J92" s="9"/>
       <c r="K92" s="25"/>
     </row>
-    <row r="93" spans="2:11">
+    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B93" s="7" t="s">
         <v>4</v>
       </c>
@@ -1973,7 +2028,7 @@
       <c r="J93" s="9"/>
       <c r="K93" s="25"/>
     </row>
-    <row r="94" spans="2:11">
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="7" t="s">
         <v>77</v>
       </c>
@@ -1986,7 +2041,7 @@
       <c r="J94" s="9"/>
       <c r="K94" s="25"/>
     </row>
-    <row r="95" spans="2:11">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="7" t="s">
         <v>67</v>
       </c>
@@ -1999,7 +2054,7 @@
       <c r="J95" s="9"/>
       <c r="K95" s="25"/>
     </row>
-    <row r="96" spans="2:11">
+    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B96" s="14" t="s">
         <v>57</v>
       </c>
@@ -2009,7 +2064,7 @@
       <c r="J96" s="9"/>
       <c r="K96" s="25"/>
     </row>
-    <row r="97" spans="2:11">
+    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B97" s="14" t="s">
         <v>58</v>
       </c>
@@ -2021,13 +2076,13 @@
       <c r="J97" s="9"/>
       <c r="K97" s="25"/>
     </row>
-    <row r="98" spans="2:11">
+    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H98" s="25"/>
       <c r="I98" s="9"/>
       <c r="J98" s="9"/>
       <c r="K98" s="25"/>
     </row>
-    <row r="99" spans="2:11">
+    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B99" s="10" t="s">
         <v>32</v>
       </c>
@@ -2042,7 +2097,7 @@
       </c>
       <c r="F99" s="22"/>
     </row>
-    <row r="100" spans="2:11">
+    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B100" s="23" t="s">
         <v>56</v>
       </c>
@@ -2051,15 +2106,15 @@
       </c>
       <c r="D100" s="23"/>
     </row>
-    <row r="101" spans="2:11">
-      <c r="B101" s="36" t="s">
+    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B101" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C101" s="36"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
-    </row>
-    <row r="102" spans="2:11">
+      <c r="C101" s="37"/>
+      <c r="D101" s="37"/>
+      <c r="E101" s="37"/>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B102" s="24"/>
       <c r="C102" s="5" t="s">
         <v>31</v>
@@ -2071,7 +2126,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="2:11">
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B103" s="14" t="s">
         <v>40</v>
       </c>
@@ -2085,7 +2140,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="104" spans="2:11">
+    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B104" s="14" t="s">
         <v>42</v>
       </c>
@@ -2093,7 +2148,7 @@
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
     </row>
-    <row r="105" spans="2:11">
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B105" s="14" t="s">
         <v>20</v>
       </c>
@@ -2103,7 +2158,7 @@
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
     </row>
-    <row r="106" spans="2:11">
+    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B106" s="14" t="s">
         <v>21</v>
       </c>
@@ -2113,7 +2168,7 @@
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
     </row>
-    <row r="107" spans="2:11">
+    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B107" s="14" t="s">
         <v>44</v>
       </c>
@@ -2123,7 +2178,7 @@
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
     </row>
-    <row r="108" spans="2:11">
+    <row r="108" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B108" s="26" t="s">
         <v>45</v>
       </c>
@@ -2135,7 +2190,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="109" spans="2:11">
+    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B109" s="26" t="s">
         <v>47</v>
       </c>
@@ -2143,14 +2198,14 @@
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
     </row>
-    <row r="110" spans="2:11">
-      <c r="B110" s="36" t="s">
+    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B110" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C110" s="36"/>
-      <c r="D110" s="36"/>
-    </row>
-    <row r="111" spans="2:11">
+      <c r="C110" s="37"/>
+      <c r="D110" s="37"/>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B111" s="5" t="s">
         <v>9</v>
       </c>
@@ -2173,7 +2228,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="112" spans="2:11">
+    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B112" s="7" t="s">
         <v>6</v>
       </c>
@@ -2192,14 +2247,14 @@
         <v>66</v>
       </c>
     </row>
-    <row r="113" spans="2:6">
-      <c r="B113" s="36" t="s">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B113" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C113" s="36"/>
-      <c r="D113" s="36"/>
-    </row>
-    <row r="114" spans="2:6">
+      <c r="C113" s="37"/>
+      <c r="D113" s="37"/>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B114" s="5" t="s">
         <v>9</v>
       </c>
@@ -2216,7 +2271,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="115" spans="2:6">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B115" s="7" t="s">
         <v>5</v>
       </c>
@@ -2229,7 +2284,7 @@
       <c r="E115" s="7"/>
       <c r="F115" s="8"/>
     </row>
-    <row r="116" spans="2:6">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B116" s="7" t="s">
         <v>4</v>
       </c>
@@ -2242,7 +2297,7 @@
       </c>
       <c r="F116" s="8"/>
     </row>
-    <row r="117" spans="2:6">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B117" s="14" t="s">
         <v>57</v>
       </c>
@@ -2250,7 +2305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="2:6">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B118" s="14" t="s">
         <v>58</v>
       </c>
@@ -2258,24 +2313,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="2:6">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B120" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="2:6">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B121" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="122" spans="2:6">
-      <c r="B122" s="36" t="s">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B122" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="C122" s="36"/>
-      <c r="D122" s="36"/>
-    </row>
-    <row r="123" spans="2:6">
+      <c r="C122" s="37"/>
+      <c r="D122" s="37"/>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B123" s="11" t="s">
         <v>76</v>
       </c>
@@ -2284,32 +2339,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="2:6">
-      <c r="B124" s="36" t="s">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B124" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C124" s="36"/>
-      <c r="D124" s="36"/>
-    </row>
-    <row r="125" spans="2:6">
-      <c r="B125" s="37" t="s">
+      <c r="C124" s="37"/>
+      <c r="D124" s="37"/>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B125" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="C125" s="38"/>
+      <c r="C125" s="49"/>
       <c r="D125" s="34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="126" spans="2:6">
-      <c r="B126" s="37" t="s">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B126" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="C126" s="38"/>
+      <c r="C126" s="49"/>
       <c r="D126" s="34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="128" spans="2:6">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B128" s="10" t="s">
         <v>32</v>
       </c>
@@ -2321,7 +2376,7 @@
       </c>
       <c r="F128" s="22"/>
     </row>
-    <row r="129" spans="2:8">
+    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B129" s="23" t="s">
         <v>68</v>
       </c>
@@ -2329,15 +2384,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="2:8">
-      <c r="B130" s="36" t="s">
+    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B130" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C130" s="36"/>
-      <c r="D130" s="36"/>
-      <c r="E130" s="36"/>
-    </row>
-    <row r="131" spans="2:8">
+      <c r="C130" s="37"/>
+      <c r="D130" s="37"/>
+      <c r="E130" s="37"/>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B131" s="24"/>
       <c r="C131" s="5" t="s">
         <v>31</v>
@@ -2349,7 +2404,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="132" spans="2:8">
+    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B132" s="14" t="s">
         <v>40</v>
       </c>
@@ -2359,7 +2414,7 @@
       </c>
       <c r="E132" s="7"/>
     </row>
-    <row r="133" spans="2:8">
+    <row r="133" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B133" s="14" t="s">
         <v>42</v>
       </c>
@@ -2367,7 +2422,7 @@
       <c r="D133" s="7"/>
       <c r="E133" s="7"/>
     </row>
-    <row r="134" spans="2:8">
+    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B134" s="14" t="s">
         <v>20</v>
       </c>
@@ -2377,7 +2432,7 @@
       </c>
       <c r="E134" s="7"/>
     </row>
-    <row r="135" spans="2:8">
+    <row r="135" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B135" s="14" t="s">
         <v>21</v>
       </c>
@@ -2387,7 +2442,7 @@
       </c>
       <c r="E135" s="7"/>
     </row>
-    <row r="136" spans="2:8">
+    <row r="136" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B136" s="14" t="s">
         <v>44</v>
       </c>
@@ -2397,11 +2452,11 @@
       <c r="D136" s="7"/>
       <c r="E136" s="7"/>
     </row>
-    <row r="137" spans="2:8">
-      <c r="B137" s="39" t="s">
+    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B137" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="C137" s="39"/>
+      <c r="C137" s="50"/>
       <c r="D137" s="7" t="s">
         <v>46</v>
       </c>
@@ -2409,7 +2464,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="138" spans="2:8">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B138" s="26" t="s">
         <v>47</v>
       </c>
@@ -2417,14 +2472,14 @@
       <c r="D138" s="7"/>
       <c r="E138" s="7"/>
     </row>
-    <row r="139" spans="2:8">
-      <c r="B139" s="36" t="s">
+    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B139" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="C139" s="36"/>
-      <c r="D139" s="36"/>
-    </row>
-    <row r="140" spans="2:8">
+      <c r="C139" s="37"/>
+      <c r="D139" s="37"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B140" s="5" t="s">
         <v>9</v>
       </c>
@@ -2447,7 +2502,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="2:8">
+    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B141" s="7" t="s">
         <v>6</v>
       </c>
@@ -2466,14 +2521,14 @@
         <v>66</v>
       </c>
     </row>
-    <row r="142" spans="2:8">
-      <c r="B142" s="36" t="s">
+    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B142" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C142" s="36"/>
-      <c r="D142" s="36"/>
-    </row>
-    <row r="143" spans="2:8">
+      <c r="C142" s="37"/>
+      <c r="D142" s="37"/>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B143" s="5" t="s">
         <v>9</v>
       </c>
@@ -2490,7 +2545,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="144" spans="2:8">
+    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B144" s="7" t="s">
         <v>5</v>
       </c>
@@ -2503,7 +2558,7 @@
       <c r="E144" s="7"/>
       <c r="F144" s="8"/>
     </row>
-    <row r="145" spans="2:6">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B145" s="7" t="s">
         <v>4</v>
       </c>
@@ -2514,7 +2569,7 @@
       <c r="E145" s="7"/>
       <c r="F145" s="8"/>
     </row>
-    <row r="146" spans="2:6">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B146" s="14" t="s">
         <v>57</v>
       </c>
@@ -2522,7 +2577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="2:6">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B147" s="14" t="s">
         <v>58</v>
       </c>
@@ -2533,16 +2588,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="23">
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B78:E78"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C4:F5"/>
-    <mergeCell ref="B4:B5"/>
     <mergeCell ref="B139:D139"/>
     <mergeCell ref="B142:D142"/>
     <mergeCell ref="B87:D87"/>
@@ -2556,6 +2601,16 @@
     <mergeCell ref="B125:C125"/>
     <mergeCell ref="B126:C126"/>
     <mergeCell ref="B137:C137"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C4:F5"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2575,69 +2630,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="28" customWidth="1"/>
     <col min="2" max="2" width="106.42578125" customWidth="1"/>
     <col min="3" max="3" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" s="29" t="str">
         <f>"&lt;forecast seriesName="&amp;CHAR(34)&amp;Schedules!D2&amp;CHAR(34)&amp;"&gt;"</f>
         <v>&lt;forecast seriesName="Influenza"&gt;</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 218, 219"/&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 217, 218, 219, 220, 221, 222"/&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B6&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C6&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Nasal" vaccineIds="180, 203"/&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Live" vaccineIds="158, 159, 160, 161, 162, 171, 175, 178, 2020"/&gt;</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B8&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C8&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="H1N1" vaccineIds="186, 187, 188, 189"/&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B9&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C9&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;vaccine vaccineName="Season Start" vaccineIds="-503"/&gt;</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" s="29" t="str">
         <f>"  &lt;seasonal due="&amp;CHAR(34)&amp;Schedules!I17&amp;CHAR(34)&amp;" overdue="&amp;CHAR(34)&amp;Schedules!I18&amp;CHAR(34)&amp;" end="&amp;CHAR(34)&amp;Schedules!I16&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;seasonal due="1 month" overdue="5 months" end="6 months"/&gt;</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="29" t="str">
         <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B34&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C34&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;transition name="" age="" vaccineId=""/&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v xml:space="preserve">  &lt;transition name="influenza injectable MDCK quadrivalent" age="" vaccineId=""/&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="str">
         <f>Schedules!B77</f>
         <v>P1</v>
@@ -2647,91 +2702,91 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="season"&gt;</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="29" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="32" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="32" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="32" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="str">
         <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B89&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C89&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E89&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F89&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G89&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H89&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B92&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F92&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B93&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F93&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B94&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F94&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E94&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="H1N1" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B95&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F95&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Season Start" schedule="S1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="32" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="str">
         <f>Schedules!B100</f>
         <v>S1</v>
@@ -2741,79 +2796,79 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="S1" dose="1" indication="" label="current season"&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="32" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C117&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="3"/&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="32" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="32" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="32" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C105&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="32" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="32" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="32" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="32" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="32" t="str">
         <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B112&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C112&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E112&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F112&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G112&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H112&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B115&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C115&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D115&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F115&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E115&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" s="32" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B116&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D116&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F116&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E116&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="DL FLU 2015" age="" reason="" seasonCompleted="Yes"/&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B36" s="32" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="str">
         <f>Schedules!B121</f>
         <v>DL FLU 2015</v>
@@ -2823,30 +2878,30 @@
         <v xml:space="preserve">  &lt;decisionLogic name="DL FLU 2015"&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="32" t="str">
         <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B123&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D123&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Flu"/&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="32" t="str">
         <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B125&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D125&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Second Dose Needed" value="S2"/&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="32" t="str">
         <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B126&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="No More Doses Needed" value="COMPLETE"/&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" s="32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="str">
         <f>Schedules!B129</f>
         <v>S2</v>
@@ -2856,79 +2911,79 @@
         <v xml:space="preserve">  &lt;schedule scheduleName="S2" dose="2" indication="" label="2nd seasonal"&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="29" t="str">
         <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C147&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C146&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="32" t="str">
         <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E132&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="32" t="str">
         <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="32" t="str">
         <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="1 month" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="32" t="str">
         <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="32" t="str">
         <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="32" t="str">
         <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
-    <row r="50" spans="2:2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="32" t="str">
         <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="32" t="str">
         <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B141&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C141&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D141&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E141&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F141&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G141&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H141&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
-    <row r="52" spans="2:2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" s="33" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B144&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F144&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H144&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E144&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="53" spans="2:2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" s="33" t="str">
         <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B145&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D145&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F145&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H145&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E145&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="COMPLETE" age="" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
-    <row r="54" spans="2:2">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B54" s="32" t="str">
         <f>"  &lt;/schedule&gt;"</f>
         <v xml:space="preserve">  &lt;/schedule&gt;</v>
       </c>
     </row>
-    <row r="55" spans="2:2">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B55" s="29" t="str">
         <f>"&lt;/forecast&gt;"</f>
         <v>&lt;/forecast&gt;</v>

</xml_diff>

<commit_message>
Update influenza schedule with changes for mappings
</commit_message>
<xml_diff>
--- a/schedules/Influenza.xlsx
+++ b/schedules/Influenza.xlsx
@@ -9,23 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15390" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358"/>
+    <workbookView xWindow="16695" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$146</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$98</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$98</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$147</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$99</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$99</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="94">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -288,19 +288,25 @@
     <t>Flucelvax, injectable, quadrivalent, preservative free</t>
   </si>
   <si>
-    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 217, 218, 219, 220, 221, 222</t>
-  </si>
-  <si>
     <t>influenza, intradermal, quadrivalent, preservative free</t>
   </si>
   <si>
-    <t>influenza nasal, unspecified formulation</t>
-  </si>
-  <si>
-    <t>influenza recombinant quadrivalent</t>
-  </si>
-  <si>
-    <t>influenza injectable MDCK quadrivalent</t>
+    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 217, 218, 219, 220, 221, 222, 223</t>
+  </si>
+  <si>
+    <t>influenza recombinant injectable trivalent</t>
+  </si>
+  <si>
+    <t>Influenza injectable MDCK quadrivalent</t>
+  </si>
+  <si>
+    <t>Influenza recombinant quadrivalent</t>
+  </si>
+  <si>
+    <t>Influenza nasal, unspecified formulation</t>
+  </si>
+  <si>
+    <t>Influenza IIV4</t>
   </si>
 </sst>
 </file>
@@ -657,12 +663,19 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -693,13 +706,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,13 +797,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>346717</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>582084</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>121627</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1193,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IT147"/>
+  <dimension ref="A1:IT148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C4" sqref="C4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1237,83 +1243,83 @@
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
+      <c r="C4" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="47"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="45"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="40">
         <v>-503</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
@@ -1352,10 +1358,10 @@
       <c r="F14" s="7">
         <v>111</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="37"/>
+      <c r="I14" s="36"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
@@ -1527,13 +1533,17 @@
       <c r="I25" s="9"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="19"/>
+      <c r="B26" s="19" t="s">
+        <v>93</v>
+      </c>
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
       <c r="E26" s="7">
         <v>204</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7">
+        <v>161</v>
+      </c>
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
@@ -1566,7 +1576,7 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="21"/>
@@ -1608,7 +1618,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="19" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="21"/>
@@ -1622,7 +1632,7 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33" s="20"/>
       <c r="D33" s="21"/>
@@ -1636,7 +1646,7 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="21"/>
@@ -1649,6 +1659,17 @@
       <c r="I34" s="9"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="7">
+        <v>223</v>
+      </c>
+      <c r="F35" s="7">
+        <v>155</v>
+      </c>
       <c r="I35" s="9"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
@@ -1738,136 +1759,125 @@
     <row r="64" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I64" s="9"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I65" s="9"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I66" s="9"/>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I67" s="9"/>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I68" s="9"/>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I69" s="9"/>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I70" s="9"/>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I71" s="9"/>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I72" s="9"/>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I73" s="9"/>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I74" s="9"/>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I75" s="9"/>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B76" s="10" t="s">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I76" s="9"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B77" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C77" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D76" s="10" t="s">
+      <c r="D77" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E76" s="22" t="s">
+      <c r="E77" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="I76" s="9"/>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B77" s="23" t="s">
+      <c r="I77" s="9"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B78" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C77" s="23">
+      <c r="C78" s="23">
         <v>1</v>
       </c>
-      <c r="D77" s="23" t="s">
+      <c r="D78" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="I77" s="9"/>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B78" s="37" t="s">
+      <c r="I78" s="9"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B79" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
-      <c r="I78" s="9"/>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B79" s="24"/>
-      <c r="C79" s="5" t="s">
+      <c r="C79" s="36"/>
+      <c r="D79" s="36"/>
+      <c r="E79" s="36"/>
+      <c r="I79" s="9"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B80" s="24"/>
+      <c r="C80" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D80" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E79" s="5" t="s">
+      <c r="E80" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I79" s="9"/>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B80" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="I80" s="9"/>
-      <c r="J80" s="9"/>
-      <c r="K80" s="25"/>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C81" s="7"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="I81" s="9"/>
       <c r="J81" s="9"/>
       <c r="K81" s="25"/>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>16</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
-      <c r="H82" s="25"/>
       <c r="I82" s="9"/>
       <c r="J82" s="9"/>
       <c r="K82" s="25"/>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
@@ -1878,7 +1888,7 @@
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" s="14" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>43</v>
@@ -1891,13 +1901,13 @@
       <c r="K84" s="25"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B85" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C85" s="27"/>
-      <c r="D85" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="B85" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D85" s="7"/>
       <c r="E85" s="7"/>
       <c r="H85" s="25"/>
       <c r="I85" s="9"/>
@@ -1906,10 +1916,12 @@
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C86" s="27"/>
-      <c r="D86" s="7"/>
+      <c r="D86" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="E86" s="7"/>
       <c r="H86" s="25"/>
       <c r="I86" s="9"/>
@@ -1917,112 +1929,111 @@
       <c r="K86" s="25"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B87" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C87" s="37"/>
-      <c r="D87" s="37"/>
+      <c r="B87" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C87" s="27"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
       <c r="H87" s="25"/>
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
       <c r="K87" s="25"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B88" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="B88" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+      <c r="H88" s="25"/>
       <c r="I88" s="9"/>
       <c r="J88" s="9"/>
       <c r="K88" s="25"/>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B89" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D89" s="7"/>
-      <c r="E89" s="7"/>
-      <c r="F89" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G89" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H89" s="7" t="s">
-        <v>66</v>
+      <c r="B89" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="I89" s="9"/>
       <c r="J89" s="9"/>
+      <c r="K89" s="25"/>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B90" s="37" t="s">
+      <c r="B90" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H90" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I90" s="9"/>
+      <c r="J90" s="9"/>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B91" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C90" s="37"/>
-      <c r="D90" s="37"/>
-      <c r="J90" s="9"/>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B91" s="5" t="s">
+      <c r="C91" s="36"/>
+      <c r="D91" s="36"/>
+      <c r="J91" s="9"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B92" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C91" s="5" t="s">
+      <c r="C92" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D92" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E91" s="5" t="s">
+      <c r="E92" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F91" s="5" t="s">
+      <c r="F92" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J91" s="9"/>
-    </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B92" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E92" s="7"/>
-      <c r="F92" s="8"/>
       <c r="J92" s="9"/>
-      <c r="K92" s="25"/>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B93" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D93" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="E93" s="7"/>
       <c r="F93" s="8"/>
       <c r="J93" s="9"/>
@@ -2030,147 +2041,150 @@
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="7" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
-      <c r="F94" s="35"/>
+      <c r="F94" s="8"/>
       <c r="J94" s="9"/>
       <c r="K94" s="25"/>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="7" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
-      <c r="F95" s="8"/>
+      <c r="F95" s="35"/>
       <c r="J95" s="9"/>
       <c r="K95" s="25"/>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B96" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C96" s="7">
-        <v>1</v>
-      </c>
+      <c r="B96" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+      <c r="F96" s="8"/>
       <c r="J96" s="9"/>
       <c r="K96" s="25"/>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B97" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C97" s="7">
         <v>1</v>
       </c>
-      <c r="H97" s="25"/>
-      <c r="I97" s="9"/>
       <c r="J97" s="9"/>
       <c r="K97" s="25"/>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B98" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C98" s="7">
+        <v>1</v>
+      </c>
       <c r="H98" s="25"/>
       <c r="I98" s="9"/>
       <c r="J98" s="9"/>
       <c r="K98" s="25"/>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B99" s="10" t="s">
+      <c r="H99" s="25"/>
+      <c r="I99" s="9"/>
+      <c r="J99" s="9"/>
+      <c r="K99" s="25"/>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B100" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C99" s="10" t="s">
+      <c r="C100" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D99" s="10" t="s">
+      <c r="D100" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E99" s="22" t="s">
+      <c r="E100" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="F99" s="22"/>
-    </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B100" s="23" t="s">
+      <c r="F100" s="22"/>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B101" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C100" s="23">
+      <c r="C101" s="23">
         <v>1</v>
       </c>
-      <c r="D100" s="23"/>
-    </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B101" s="37" t="s">
+      <c r="D101" s="23"/>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B102" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C101" s="37"/>
-      <c r="D101" s="37"/>
-      <c r="E101" s="37"/>
-    </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B102" s="24"/>
-      <c r="C102" s="5" t="s">
+      <c r="C102" s="36"/>
+      <c r="D102" s="36"/>
+      <c r="E102" s="36"/>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B103" s="24"/>
+      <c r="C103" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D103" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E102" s="5" t="s">
+      <c r="E103" s="5" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B103" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D103" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E103" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B104" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C104" s="7"/>
-      <c r="D104" s="7"/>
-      <c r="E104" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B105" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C105" s="7" t="s">
-        <v>16</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B106" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B107" s="14" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>43</v>
@@ -2179,438 +2193,448 @@
       <c r="E107" s="7"/>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B108" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C108" s="27"/>
-      <c r="D108" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E108" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="B108" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B109" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C109" s="27"/>
+      <c r="D109" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B110" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C109" s="27"/>
-      <c r="D109" s="7"/>
-      <c r="E109" s="7"/>
-    </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B110" s="37" t="s">
+      <c r="C110" s="27"/>
+      <c r="D110" s="7"/>
+      <c r="E110" s="7"/>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B111" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C110" s="37"/>
-      <c r="D110" s="37"/>
-    </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B111" s="5" t="s">
+      <c r="C111" s="36"/>
+      <c r="D111" s="36"/>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B112" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C111" s="5" t="s">
+      <c r="C112" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="D112" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E111" s="5" t="s">
+      <c r="E112" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F111" s="5" t="s">
+      <c r="F112" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G111" s="5" t="s">
+      <c r="G112" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H111" s="5" t="s">
+      <c r="H112" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B112" s="7" t="s">
+    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B113" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C112" s="7" t="s">
+      <c r="C113" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-      <c r="F112" s="7" t="s">
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G112" s="7" t="s">
+      <c r="G113" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H112" s="7" t="s">
+      <c r="H113" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B113" s="37" t="s">
+    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B114" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C113" s="37"/>
-      <c r="D113" s="37"/>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B114" s="5" t="s">
+      <c r="C114" s="36"/>
+      <c r="D114" s="36"/>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B115" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C114" s="5" t="s">
+      <c r="C115" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D115" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E114" s="5" t="s">
+      <c r="E115" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F114" s="5" t="s">
+      <c r="F115" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B115" s="7" t="s">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B116" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C115" s="7" t="s">
+      <c r="C116" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D115" s="7" t="s">
+      <c r="D116" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E115" s="7"/>
-      <c r="F115" s="8"/>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B116" s="7" t="s">
+      <c r="E116" s="7"/>
+      <c r="F116" s="8"/>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B117" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C117" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D116" s="7"/>
-      <c r="E116" s="7" t="s">
+      <c r="D117" s="7"/>
+      <c r="E117" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F116" s="8"/>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B117" s="14" t="s">
+      <c r="F117" s="8"/>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B118" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C117" s="7">
+      <c r="C118" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B118" s="14" t="s">
+    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B119" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C118" s="7">
+      <c r="C119" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B120" s="10" t="s">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B121" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B121" s="4" t="s">
+    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B122" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B122" s="37" t="s">
+    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B123" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C122" s="37"/>
-      <c r="D122" s="37"/>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B123" s="11" t="s">
+      <c r="C123" s="36"/>
+      <c r="D123" s="36"/>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B124" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C123" s="13"/>
-      <c r="D123" s="34" t="s">
+      <c r="C124" s="13"/>
+      <c r="D124" s="34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B124" s="37" t="s">
+    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B125" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C124" s="37"/>
-      <c r="D124" s="37"/>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B125" s="48" t="s">
+      <c r="C125" s="36"/>
+      <c r="D125" s="36"/>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B126" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="C125" s="49"/>
-      <c r="D125" s="34" t="s">
+      <c r="C126" s="38"/>
+      <c r="D126" s="34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B126" s="48" t="s">
+    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B127" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="C126" s="49"/>
-      <c r="D126" s="34" t="s">
+      <c r="C127" s="38"/>
+      <c r="D127" s="34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B128" s="10" t="s">
+    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B129" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C128" s="10" t="s">
+      <c r="C129" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E128" s="22" t="s">
+      <c r="E129" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F128" s="22"/>
-    </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B129" s="23" t="s">
+      <c r="F129" s="22"/>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B130" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C129" s="23">
+      <c r="C130" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B130" s="37" t="s">
+    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B131" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C130" s="37"/>
-      <c r="D130" s="37"/>
-      <c r="E130" s="37"/>
-    </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B131" s="24"/>
-      <c r="C131" s="5" t="s">
+      <c r="C131" s="36"/>
+      <c r="D131" s="36"/>
+      <c r="E131" s="36"/>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B132" s="24"/>
+      <c r="C132" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D132" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E131" s="5" t="s">
+      <c r="E132" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B132" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C132" s="7"/>
-      <c r="D132" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E132" s="7"/>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B133" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C133" s="7"/>
-      <c r="D133" s="7"/>
+      <c r="D133" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="E133" s="7"/>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B134" s="14" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C134" s="7"/>
-      <c r="D134" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="D134" s="7"/>
       <c r="E134" s="7"/>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B135" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C135" s="7"/>
       <c r="D135" s="7" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E135" s="7"/>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B136" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C136" s="7"/>
+      <c r="D136" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E136" s="7"/>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B137" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C136" s="7" t="s">
+      <c r="C137" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D136" s="7"/>
-      <c r="E136" s="7"/>
-    </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B137" s="50" t="s">
+      <c r="D137" s="7"/>
+      <c r="E137" s="7"/>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B138" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C137" s="50"/>
-      <c r="D137" s="7" t="s">
+      <c r="C138" s="39"/>
+      <c r="D138" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E137" s="7" t="s">
+      <c r="E138" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B138" s="26" t="s">
+    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B139" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C138" s="27"/>
-      <c r="D138" s="7"/>
-      <c r="E138" s="7"/>
-    </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B139" s="37" t="s">
+      <c r="C139" s="27"/>
+      <c r="D139" s="7"/>
+      <c r="E139" s="7"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B140" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C139" s="37"/>
-      <c r="D139" s="37"/>
-    </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B140" s="5" t="s">
+      <c r="C140" s="36"/>
+      <c r="D140" s="36"/>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B141" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C140" s="5" t="s">
+      <c r="C141" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D140" s="5" t="s">
+      <c r="D141" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E140" s="5" t="s">
+      <c r="E141" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F140" s="5" t="s">
+      <c r="F141" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G140" s="5" t="s">
+      <c r="G141" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H140" s="5" t="s">
+      <c r="H141" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B141" s="7" t="s">
+    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B142" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C141" s="7" t="s">
+      <c r="C142" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D141" s="7"/>
-      <c r="E141" s="7"/>
-      <c r="F141" s="7" t="s">
+      <c r="D142" s="7"/>
+      <c r="E142" s="7"/>
+      <c r="F142" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G141" s="7" t="s">
+      <c r="G142" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H141" s="7" t="s">
+      <c r="H142" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B142" s="37" t="s">
+    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B143" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C142" s="37"/>
-      <c r="D142" s="37"/>
-    </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B143" s="5" t="s">
+      <c r="C143" s="36"/>
+      <c r="D143" s="36"/>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B144" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C143" s="5" t="s">
+      <c r="C144" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D143" s="5" t="s">
+      <c r="D144" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E143" s="5" t="s">
+      <c r="E144" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F143" s="5" t="s">
+      <c r="F144" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B144" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C144" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D144" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E144" s="7"/>
-      <c r="F144" s="8"/>
     </row>
     <row r="145" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B145" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D145" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="D145" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="E145" s="7"/>
       <c r="F145" s="8"/>
     </row>
     <row r="146" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B146" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C146" s="7">
-        <v>2</v>
-      </c>
+      <c r="B146" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D146" s="7"/>
+      <c r="E146" s="7"/>
+      <c r="F146" s="8"/>
     </row>
     <row r="147" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B147" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C147" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B148" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C147" s="7">
+      <c r="C148" s="7">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="23">
-    <mergeCell ref="B139:D139"/>
-    <mergeCell ref="B142:D142"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B101:E101"/>
-    <mergeCell ref="B110:D110"/>
-    <mergeCell ref="B113:D113"/>
-    <mergeCell ref="B130:E130"/>
-    <mergeCell ref="B122:D122"/>
-    <mergeCell ref="B124:D124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B137:C137"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B79:E79"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C4:F5"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B140:D140"/>
+    <mergeCell ref="B143:D143"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B102:E102"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="B131:E131"/>
+    <mergeCell ref="B123:D123"/>
+    <mergeCell ref="B125:D125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B138:C138"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2620,10 +2644,10 @@
     <oddFooter>&amp;CPrepared by  Nathan Bunker &amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <rowBreaks count="4" manualBreakCount="4">
-    <brk id="35" max="16383" man="1"/>
-    <brk id="75" max="16383" man="1"/>
-    <brk id="98" max="16383" man="1"/>
-    <brk id="127" max="16383" man="1"/>
+    <brk id="36" max="16383" man="1"/>
+    <brk id="76" max="16383" man="1"/>
+    <brk id="99" max="16383" man="1"/>
+    <brk id="128" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -2653,7 +2677,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 217, 218, 219, 220, 221, 222"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 217, 218, 219, 220, 221, 222, 223"/&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2689,94 +2713,94 @@
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="29" t="str">
         <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B34&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C34&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;transition name="influenza injectable MDCK quadrivalent" age="" vaccineId=""/&gt;</v>
+        <v xml:space="preserve">  &lt;transition name="Influenza injectable MDCK quadrivalent" age="" vaccineId=""/&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="str">
-        <f>Schedules!B77</f>
+        <f>Schedules!B78</f>
         <v>P1</v>
       </c>
       <c r="B9" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B77&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C77&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D77&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E76&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B78&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C78&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D78&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E77&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="season"&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C85&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D87&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B89&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C89&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E89&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F89&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G89&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H89&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B90&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C90&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F90&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G90&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H90&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B92&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F92&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B93&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F93&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B93&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F93&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B94&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F94&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E94&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B94&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F94&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E94&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B95&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F95&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="H1N1" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B95&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F95&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B96&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D96&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F96&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E96&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Season Start" schedule="S1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
@@ -2788,77 +2812,77 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="str">
-        <f>Schedules!B100</f>
+        <f>Schedules!B101</f>
         <v>S1</v>
       </c>
       <c r="B24" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B100&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D100&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E99&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B101&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D101&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E100&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S1" dose="1" indication="" label="current season"&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="32" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C117&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C119&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="3"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C105&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C105&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C108&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E109&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D110&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B112&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C112&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E112&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F112&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G112&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H112&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B113&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C113&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D113&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E113&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F113&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G113&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H113&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B115&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C115&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D115&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F115&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E115&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B116&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D116&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F116&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E116&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B116&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D116&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F116&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E116&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B117&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C117&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D117&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F117&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E117&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="DL FLU 2015" age="" reason="" seasonCompleted="Yes"/&gt;</v>
       </c>
     </row>
@@ -2870,29 +2894,29 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="str">
-        <f>Schedules!B121</f>
+        <f>Schedules!B122</f>
         <v>DL FLU 2015</v>
       </c>
       <c r="B37" s="31" t="str">
-        <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B121&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B122&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;decisionLogic name="DL FLU 2015"&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="32" t="str">
-        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B123&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D123&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B124&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D124&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Flu"/&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B125&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D125&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B126&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Second Dose Needed" value="S2"/&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B126&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B127&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="No More Doses Needed" value="COMPLETE"/&gt;</v>
       </c>
     </row>
@@ -2903,77 +2927,77 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="str">
-        <f>Schedules!B129</f>
+        <f>Schedules!B130</f>
         <v>S2</v>
       </c>
       <c r="B42" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B129&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C129&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D129&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E128&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B130&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C130&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D130&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E129&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S2" dose="2" indication="" label="2nd seasonal"&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C147&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C146&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C148&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C147&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E132&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="1 month" grace=""/&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C137&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E138&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D139&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B141&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C141&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D141&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E141&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F141&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G141&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H141&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B142&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C142&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D142&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E142&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F142&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G142&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H142&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B144&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F144&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H144&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E144&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B145&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D145&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F145&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H145&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E145&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B145&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D145&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F145&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H145&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E145&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B146&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C146&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D146&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F146&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H146&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E146&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="COMPLETE" age="" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add support for TCH Vaccine ID 205 flu
This is part of the new mapping for CVX 158 <-> TCH Vaccine ID 205
</commit_message>
<xml_diff>
--- a/schedules/Influenza.xlsx
+++ b/schedules/Influenza.xlsx
@@ -9,23 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16695" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358"/>
+    <workbookView xWindow="19305" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$147</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$99</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$99</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$149</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$101</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$101</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="94">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -291,9 +291,6 @@
     <t>influenza, intradermal, quadrivalent, preservative free</t>
   </si>
   <si>
-    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 217, 218, 219, 220, 221, 222, 223</t>
-  </si>
-  <si>
     <t>influenza recombinant injectable trivalent</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>Influenza IIV4</t>
+  </si>
+  <si>
+    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 205, 204, 203, 202, 217, 218, 219, 220, 221, 222, 223</t>
   </si>
 </sst>
 </file>
@@ -797,14 +797,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>346717</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>84667</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>582084</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>121627</xdr:rowOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>36960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1199,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IT148"/>
+  <dimension ref="A1:IT150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F5"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1255,7 +1255,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
@@ -1534,99 +1534,99 @@
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
       <c r="E26" s="7">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F26" s="7">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I26" s="9"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="19" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
       <c r="E27" s="7">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F27" s="7">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="21"/>
       <c r="E28" s="7">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F28" s="7">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="21"/>
       <c r="E29" s="7">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="F29" s="7">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="21"/>
       <c r="E30" s="7">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F30" s="7">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I30" s="9"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" s="20"/>
       <c r="D31" s="21"/>
       <c r="E31" s="7">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F31" s="7">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I31" s="9"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="19" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="21"/>
       <c r="E32" s="7">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F32" s="7">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="I32" s="9"/>
     </row>
@@ -1637,10 +1637,10 @@
       <c r="C33" s="20"/>
       <c r="D33" s="21"/>
       <c r="E33" s="7">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F33" s="7">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="I33" s="9"/>
     </row>
@@ -1651,10 +1651,10 @@
       <c r="C34" s="20"/>
       <c r="D34" s="21"/>
       <c r="E34" s="7">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F34" s="7">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I34" s="9"/>
     </row>
@@ -1665,14 +1665,25 @@
       <c r="C35" s="20"/>
       <c r="D35" s="21"/>
       <c r="E35" s="7">
+        <v>222</v>
+      </c>
+      <c r="F35" s="7">
+        <v>186</v>
+      </c>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="7">
         <v>223</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F36" s="7">
         <v>155</v>
       </c>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="I36" s="9"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
@@ -1796,116 +1807,94 @@
       <c r="I76" s="9"/>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B77" s="10" t="s">
+      <c r="I77" s="9"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I78" s="9"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B79" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C77" s="10" t="s">
+      <c r="C79" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D77" s="10" t="s">
+      <c r="D79" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E77" s="22" t="s">
+      <c r="E79" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="I77" s="9"/>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B78" s="23" t="s">
+      <c r="I79" s="9"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B80" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C78" s="23">
+      <c r="C80" s="23">
         <v>1</v>
       </c>
-      <c r="D78" s="23" t="s">
+      <c r="D80" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="I78" s="9"/>
-    </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B79" s="36" t="s">
+      <c r="I80" s="9"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B81" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="36"/>
-      <c r="I79" s="9"/>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B80" s="24"/>
-      <c r="C80" s="5" t="s">
+      <c r="C81" s="36"/>
+      <c r="D81" s="36"/>
+      <c r="E81" s="36"/>
+      <c r="I81" s="9"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B82" s="24"/>
+      <c r="C82" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D82" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E80" s="5" t="s">
+      <c r="E82" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I80" s="9"/>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B81" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I81" s="9"/>
-      <c r="J81" s="9"/>
-      <c r="K81" s="25"/>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B82" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
       <c r="I82" s="9"/>
-      <c r="J82" s="9"/>
-      <c r="K82" s="25"/>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" s="14" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
-      <c r="H83" s="25"/>
+      <c r="D83" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="I83" s="9"/>
       <c r="J83" s="9"/>
       <c r="K83" s="25"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
-      <c r="H84" s="25"/>
       <c r="I84" s="9"/>
       <c r="J84" s="9"/>
       <c r="K84" s="25"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" s="14" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
@@ -1915,13 +1904,13 @@
       <c r="K85" s="25"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B86" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C86" s="27"/>
-      <c r="D86" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="B86" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D86" s="7"/>
       <c r="E86" s="7"/>
       <c r="H86" s="25"/>
       <c r="I86" s="9"/>
@@ -1929,10 +1918,12 @@
       <c r="K86" s="25"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B87" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C87" s="27"/>
+      <c r="B87" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="H87" s="25"/>
@@ -1941,136 +1932,136 @@
       <c r="K87" s="25"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B88" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="C88" s="36"/>
-      <c r="D88" s="36"/>
+      <c r="B88" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C88" s="27"/>
+      <c r="D88" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E88" s="7"/>
       <c r="H88" s="25"/>
       <c r="I88" s="9"/>
       <c r="J88" s="9"/>
       <c r="K88" s="25"/>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B89" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="B89" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C89" s="27"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="H89" s="25"/>
       <c r="I89" s="9"/>
       <c r="J89" s="9"/>
       <c r="K89" s="25"/>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B90" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D90" s="7"/>
-      <c r="E90" s="7"/>
-      <c r="F90" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G90" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="B90" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C90" s="36"/>
+      <c r="D90" s="36"/>
+      <c r="H90" s="25"/>
       <c r="I90" s="9"/>
       <c r="J90" s="9"/>
+      <c r="K90" s="25"/>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B91" s="36" t="s">
+      <c r="B91" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I91" s="9"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="25"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B92" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H92" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I92" s="9"/>
+      <c r="J92" s="9"/>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B93" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C91" s="36"/>
-      <c r="D91" s="36"/>
-      <c r="J91" s="9"/>
-    </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B92" s="5" t="s">
+      <c r="C93" s="36"/>
+      <c r="D93" s="36"/>
+      <c r="J93" s="9"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B94" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C92" s="5" t="s">
+      <c r="C94" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D94" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E94" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="F94" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J92" s="9"/>
-    </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B93" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E93" s="7"/>
-      <c r="F93" s="8"/>
-      <c r="J93" s="9"/>
-      <c r="K93" s="25"/>
-    </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B94" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D94" s="7"/>
-      <c r="E94" s="7"/>
-      <c r="F94" s="8"/>
       <c r="J94" s="9"/>
-      <c r="K94" s="25"/>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="7" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D95" s="7"/>
+        <v>54</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="E95" s="7"/>
-      <c r="F95" s="35"/>
+      <c r="F95" s="8"/>
       <c r="J95" s="9"/>
       <c r="K95" s="25"/>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B96" s="7" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="7"/>
@@ -2079,533 +2070,559 @@
       <c r="K96" s="25"/>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B97" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C97" s="7">
-        <v>1</v>
-      </c>
+      <c r="B97" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="35"/>
       <c r="J97" s="9"/>
       <c r="K97" s="25"/>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B98" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C98" s="7">
-        <v>1</v>
-      </c>
-      <c r="H98" s="25"/>
-      <c r="I98" s="9"/>
+      <c r="B98" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="8"/>
       <c r="J98" s="9"/>
       <c r="K98" s="25"/>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H99" s="25"/>
-      <c r="I99" s="9"/>
+      <c r="B99" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C99" s="7">
+        <v>1</v>
+      </c>
       <c r="J99" s="9"/>
       <c r="K99" s="25"/>
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B100" s="10" t="s">
+      <c r="B100" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C100" s="7">
+        <v>1</v>
+      </c>
+      <c r="H100" s="25"/>
+      <c r="I100" s="9"/>
+      <c r="J100" s="9"/>
+      <c r="K100" s="25"/>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H101" s="25"/>
+      <c r="I101" s="9"/>
+      <c r="J101" s="9"/>
+      <c r="K101" s="25"/>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B102" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C100" s="10" t="s">
+      <c r="C102" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D100" s="10" t="s">
+      <c r="D102" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E100" s="22" t="s">
+      <c r="E102" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="F100" s="22"/>
-    </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B101" s="23" t="s">
+      <c r="F102" s="22"/>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B103" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C101" s="23">
+      <c r="C103" s="23">
         <v>1</v>
       </c>
-      <c r="D101" s="23"/>
-    </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B102" s="36" t="s">
+      <c r="D103" s="23"/>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B104" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C102" s="36"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="36"/>
-    </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B103" s="24"/>
-      <c r="C103" s="5" t="s">
+      <c r="C104" s="36"/>
+      <c r="D104" s="36"/>
+      <c r="E104" s="36"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B105" s="24"/>
+      <c r="C105" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D105" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E103" s="5" t="s">
+      <c r="E105" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B104" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C104" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E104" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B105" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C105" s="7"/>
-      <c r="D105" s="7"/>
-      <c r="E105" s="7"/>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B106" s="14" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D106" s="7"/>
-      <c r="E106" s="7"/>
+      <c r="D106" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B107" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C107" s="7" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B108" s="14" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B109" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C109" s="27"/>
-      <c r="D109" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E109" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="B109" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
     </row>
     <row r="110" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B110" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C110" s="27"/>
+      <c r="B110" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B111" s="36" t="s">
+      <c r="B111" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C111" s="27"/>
+      <c r="D111" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B112" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C112" s="27"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B113" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C111" s="36"/>
-      <c r="D111" s="36"/>
-    </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B112" s="5" t="s">
+      <c r="C113" s="36"/>
+      <c r="D113" s="36"/>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B114" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C112" s="5" t="s">
+      <c r="C114" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="D114" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E112" s="5" t="s">
+      <c r="E114" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F112" s="5" t="s">
+      <c r="F114" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G112" s="5" t="s">
+      <c r="G114" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H112" s="5" t="s">
+      <c r="H114" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B113" s="7" t="s">
+    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B115" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C113" s="7" t="s">
+      <c r="C115" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
-      <c r="F113" s="7" t="s">
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G113" s="7" t="s">
+      <c r="G115" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H113" s="7" t="s">
+      <c r="H115" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B114" s="36" t="s">
+    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B116" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C114" s="36"/>
-      <c r="D114" s="36"/>
-    </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B115" s="5" t="s">
+      <c r="C116" s="36"/>
+      <c r="D116" s="36"/>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B117" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C115" s="5" t="s">
+      <c r="C117" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="D117" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E115" s="5" t="s">
+      <c r="E117" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F115" s="5" t="s">
+      <c r="F117" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B116" s="7" t="s">
+    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B118" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C116" s="7" t="s">
+      <c r="C118" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D116" s="7" t="s">
+      <c r="D118" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E116" s="7"/>
-      <c r="F116" s="8"/>
-    </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B117" s="7" t="s">
+      <c r="E118" s="7"/>
+      <c r="F118" s="8"/>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B119" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C117" s="7" t="s">
+      <c r="C119" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D117" s="7"/>
-      <c r="E117" s="7" t="s">
+      <c r="D119" s="7"/>
+      <c r="E119" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F117" s="8"/>
-    </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B118" s="14" t="s">
+      <c r="F119" s="8"/>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B120" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C118" s="7">
+      <c r="C120" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B119" s="14" t="s">
+    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B121" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C119" s="7">
+      <c r="C121" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B121" s="10" t="s">
+    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B123" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B122" s="4" t="s">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B124" s="4" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B123" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C123" s="36"/>
-      <c r="D123" s="36"/>
-    </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B124" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C124" s="13"/>
-      <c r="D124" s="34" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="125" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B125" s="36" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="C125" s="36"/>
       <c r="D125" s="36"/>
     </row>
     <row r="126" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B126" s="37" t="s">
+      <c r="B126" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C126" s="13"/>
+      <c r="D126" s="34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B127" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C127" s="36"/>
+      <c r="D127" s="36"/>
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B128" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="C126" s="38"/>
-      <c r="D126" s="34" t="s">
+      <c r="C128" s="38"/>
+      <c r="D128" s="34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B127" s="37" t="s">
+    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B129" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="C127" s="38"/>
-      <c r="D127" s="34" t="s">
+      <c r="C129" s="38"/>
+      <c r="D129" s="34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B129" s="10" t="s">
+    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B131" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C129" s="10" t="s">
+      <c r="C131" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E129" s="22" t="s">
+      <c r="E131" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F129" s="22"/>
-    </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B130" s="23" t="s">
+      <c r="F131" s="22"/>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B132" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C130" s="23">
+      <c r="C132" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B131" s="36" t="s">
+    <row r="133" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B133" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C131" s="36"/>
-      <c r="D131" s="36"/>
-      <c r="E131" s="36"/>
-    </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B132" s="24"/>
-      <c r="C132" s="5" t="s">
+      <c r="C133" s="36"/>
+      <c r="D133" s="36"/>
+      <c r="E133" s="36"/>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B134" s="24"/>
+      <c r="C134" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D134" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E132" s="5" t="s">
+      <c r="E134" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B133" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C133" s="7"/>
-      <c r="D133" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E133" s="7"/>
-    </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B134" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C134" s="7"/>
-      <c r="D134" s="7"/>
-      <c r="E134" s="7"/>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B135" s="14" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C135" s="7"/>
       <c r="D135" s="7" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E135" s="7"/>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B136" s="14" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C136" s="7"/>
-      <c r="D136" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="D136" s="7"/>
       <c r="E136" s="7"/>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B137" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C137" s="7"/>
+      <c r="D137" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E137" s="7"/>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B138" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C138" s="7"/>
+      <c r="D138" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E138" s="7"/>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B139" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C137" s="7" t="s">
+      <c r="C139" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D137" s="7"/>
-      <c r="E137" s="7"/>
-    </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B138" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="C138" s="39"/>
-      <c r="D138" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E138" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B139" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C139" s="27"/>
       <c r="D139" s="7"/>
       <c r="E139" s="7"/>
     </row>
     <row r="140" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B140" s="36" t="s">
+      <c r="B140" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C140" s="39"/>
+      <c r="D140" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E140" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B141" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C141" s="27"/>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B142" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C140" s="36"/>
-      <c r="D140" s="36"/>
-    </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B141" s="5" t="s">
+      <c r="C142" s="36"/>
+      <c r="D142" s="36"/>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B143" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C141" s="5" t="s">
+      <c r="C143" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D141" s="5" t="s">
+      <c r="D143" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E141" s="5" t="s">
+      <c r="E143" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F141" s="5" t="s">
+      <c r="F143" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G141" s="5" t="s">
+      <c r="G143" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H141" s="5" t="s">
+      <c r="H143" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B142" s="7" t="s">
+    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B144" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C142" s="7" t="s">
+      <c r="C144" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D142" s="7"/>
-      <c r="E142" s="7"/>
-      <c r="F142" s="7" t="s">
+      <c r="D144" s="7"/>
+      <c r="E144" s="7"/>
+      <c r="F144" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G142" s="7" t="s">
+      <c r="G144" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H142" s="7" t="s">
+      <c r="H144" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B143" s="36" t="s">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B145" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C143" s="36"/>
-      <c r="D143" s="36"/>
-    </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B144" s="5" t="s">
+      <c r="C145" s="36"/>
+      <c r="D145" s="36"/>
+    </row>
+    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B146" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C144" s="5" t="s">
+      <c r="C146" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D144" s="5" t="s">
+      <c r="D146" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E144" s="5" t="s">
+      <c r="E146" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F144" s="5" t="s">
+      <c r="F146" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B145" s="7" t="s">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B147" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C145" s="7" t="s">
+      <c r="C147" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D145" s="7" t="s">
+      <c r="D147" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E145" s="7"/>
-      <c r="F145" s="8"/>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B146" s="7" t="s">
+      <c r="E147" s="7"/>
+      <c r="F147" s="8"/>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B148" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C146" s="7" t="s">
+      <c r="C148" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D146" s="7"/>
-      <c r="E146" s="7"/>
-      <c r="F146" s="8"/>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B147" s="14" t="s">
+      <c r="D148" s="7"/>
+      <c r="E148" s="7"/>
+      <c r="F148" s="8"/>
+    </row>
+    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B149" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C147" s="7">
+      <c r="C149" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B148" s="14" t="s">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B150" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C148" s="7">
+      <c r="C150" s="7">
         <v>1</v>
       </c>
     </row>
@@ -2615,26 +2632,26 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B81:E81"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C4:F5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B140:D140"/>
-    <mergeCell ref="B143:D143"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B102:E102"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="B131:E131"/>
-    <mergeCell ref="B123:D123"/>
+    <mergeCell ref="B142:D142"/>
+    <mergeCell ref="B145:D145"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B133:E133"/>
     <mergeCell ref="B125:D125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B127:D127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B140:C140"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2643,11 +2660,10 @@
     <oddHeader>&amp;C&amp;F</oddHeader>
     <oddFooter>&amp;CPrepared by  Nathan Bunker &amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
-  <rowBreaks count="4" manualBreakCount="4">
-    <brk id="36" max="16383" man="1"/>
-    <brk id="76" max="16383" man="1"/>
-    <brk id="99" max="16383" man="1"/>
-    <brk id="128" max="16383" man="1"/>
+  <rowBreaks count="3" manualBreakCount="3">
+    <brk id="78" max="16383" man="1"/>
+    <brk id="101" max="16383" man="1"/>
+    <brk id="130" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -2677,7 +2693,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 204, 203, 202, 217, 218, 219, 220, 221, 222, 223"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 205, 204, 203, 202, 217, 218, 219, 220, 221, 222, 223"/&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2712,95 +2728,95 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="29" t="str">
-        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B34&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C34&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D34&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"  &lt;transition name="&amp;CHAR(34)&amp;Schedules!B35&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!C35&amp;CHAR(34)&amp;" vaccineId="&amp;CHAR(34)&amp;Schedules!D35&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">  &lt;transition name="Influenza injectable MDCK quadrivalent" age="" vaccineId=""/&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="str">
-        <f>Schedules!B78</f>
+        <f>Schedules!B80</f>
         <v>P1</v>
       </c>
       <c r="B9" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B78&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C78&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D78&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E77&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B80&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E79&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="season"&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C99&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C85&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C85&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C87&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D87&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E87&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D88&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E88&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D87&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B90&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C90&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F90&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G90&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H90&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B92&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F92&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G92&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H92&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B93&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F93&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B95&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F95&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B94&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D94&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F94&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E94&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B96&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D96&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F96&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E96&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B95&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F95&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B97&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D97&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F97&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E97&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="H1N1" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B96&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D96&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F96&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E96&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B98&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D98&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F98&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E98&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Season Start" schedule="S1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
@@ -2812,77 +2828,77 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="str">
-        <f>Schedules!B101</f>
+        <f>Schedules!B103</f>
         <v>S1</v>
       </c>
       <c r="B24" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B101&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D101&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E100&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B103&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E102&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S1" dose="1" indication="" label="current season"&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="32" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C119&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C121&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C120&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="3"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C105&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C108&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C109&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E109&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C108&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C110&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D110&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E110&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E109&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D111&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E111&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D110&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B113&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C113&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D113&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E113&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F113&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G113&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H113&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B115&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C115&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D115&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E115&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F115&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G115&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H115&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B116&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D116&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F116&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E116&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B118&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D118&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F118&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E118&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B117&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C117&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D117&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F117&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E117&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B119&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C119&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D119&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F119&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E119&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="DL FLU 2015" age="" reason="" seasonCompleted="Yes"/&gt;</v>
       </c>
     </row>
@@ -2894,29 +2910,29 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="str">
-        <f>Schedules!B122</f>
+        <f>Schedules!B124</f>
         <v>DL FLU 2015</v>
       </c>
       <c r="B37" s="31" t="str">
-        <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B122&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B124&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;decisionLogic name="DL FLU 2015"&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="32" t="str">
-        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B124&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D124&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B126&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Flu"/&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B126&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B128&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D128&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Second Dose Needed" value="S2"/&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B127&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B129&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D129&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="No More Doses Needed" value="COMPLETE"/&gt;</v>
       </c>
     </row>
@@ -2927,77 +2943,77 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="str">
-        <f>Schedules!B130</f>
+        <f>Schedules!B132</f>
         <v>S2</v>
       </c>
       <c r="B42" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B130&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C130&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D130&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E129&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B132&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E131&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S2" dose="2" indication="" label="2nd seasonal"&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C148&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C147&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C150&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C149&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E133&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C137&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="1 month" grace=""/&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C138&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E138&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C137&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C139&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D139&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E139&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E138&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D140&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E140&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D139&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D141&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B142&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C142&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D142&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E142&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F142&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G142&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H142&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B144&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E144&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F144&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G144&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H144&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B145&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D145&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F145&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H145&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E145&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B147&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C147&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D147&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F147&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H147&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E147&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B146&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C146&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D146&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F146&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H146&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E146&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B148&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C148&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D148&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F148&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H148&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E148&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="COMPLETE" age="" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Diptheria, HiB, Influenza, and Polio schedules Original date: 2018-03-04
</commit_message>
<xml_diff>
--- a/schedules/Influenza.xlsx
+++ b/schedules/Influenza.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCHWorkspaceJava6\fv\schedules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCH\TCHWorkspaces\iris006-ws\fv\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19305" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358"/>
+    <workbookView xWindow="23175" yWindow="165" windowWidth="14745" windowHeight="13110" tabRatio="358" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$149</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$101</definedName>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$101</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area">Schedules!$A$1:$L$150</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$102</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1_1">Schedules!$A$1:$L$102</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="95">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Live</t>
   </si>
   <si>
-    <t>158, 159, 160, 161, 162, 171, 175, 178, 2020</t>
-  </si>
-  <si>
     <t>Seasonal Schedule</t>
   </si>
   <si>
@@ -306,13 +303,19 @@
     <t>Influenza IIV4</t>
   </si>
   <si>
-    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 205, 204, 203, 202, 217, 218, 219, 220, 221, 222, 223</t>
+    <t>2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 205, 204, 203, 202, 217, 218, 219, 220, 221, 222, 223, 229</t>
+  </si>
+  <si>
+    <t>influenza IIV3 MDCK</t>
+  </si>
+  <si>
+    <t>180, 187, 203, 204, 220</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -663,9 +666,42 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -673,39 +709,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,18 +800,24 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>346717</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>582084</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>36960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="https://documents.lucidchart.com/documents/93c36fcd-5ce5-4343-a038-0b88849cce12/pages/0_0?a=4225&amp;x=167&amp;y=36&amp;w=935&amp;h=976&amp;store=1&amp;accept=image%2F*&amp;auth=LCA%201ccd8344df33cf5184460d1058691c59e7d5f632-ts%3D1435698127"/>
+        <xdr:cNvPr id="4" name="Picture 3" descr="https://documents.lucidchart.com/documents/93c36fcd-5ce5-4343-a038-0b88849cce12/pages/0_0?a=4225&amp;x=167&amp;y=36&amp;w=935&amp;h=976&amp;store=1&amp;accept=image%2F*&amp;auth=LCA%201ccd8344df33cf5184460d1058691c59e7d5f632-ts%3D1435698127">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1198,11 +1207,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IT150"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:IT151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="C8" sqref="C8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1243,100 +1252,100 @@
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="45"/>
+      <c r="C4" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="50"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="45"/>
     </row>
     <row r="6" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
+      <c r="C6" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
+      <c r="C7" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="40">
+        <v>66</v>
+      </c>
+      <c r="C9" s="36">
         <v>-503</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
       <c r="E12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
@@ -1348,7 +1357,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="21"/>
@@ -1358,14 +1367,14 @@
       <c r="F14" s="7">
         <v>111</v>
       </c>
-      <c r="H14" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="36"/>
+      <c r="H14" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="37"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="21"/>
@@ -1376,15 +1385,15 @@
         <v>15</v>
       </c>
       <c r="H15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="17"/>
@@ -1393,15 +1402,15 @@
       </c>
       <c r="F16" s="7"/>
       <c r="H16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
@@ -1410,10 +1419,10 @@
       </c>
       <c r="F17" s="7"/>
       <c r="H17" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
@@ -1429,15 +1438,15 @@
         <v>88</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="21"/>
@@ -1450,7 +1459,7 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21"/>
@@ -1464,7 +1473,7 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="21"/>
@@ -1478,7 +1487,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="21"/>
@@ -1492,7 +1501,7 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
@@ -1506,7 +1515,7 @@
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
@@ -1520,7 +1529,7 @@
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25" s="21"/>
@@ -1534,7 +1543,7 @@
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
@@ -1548,7 +1557,7 @@
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B27" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
@@ -1562,7 +1571,7 @@
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B28" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="21"/>
@@ -1576,7 +1585,7 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="20"/>
       <c r="D29" s="21"/>
@@ -1590,7 +1599,7 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="20"/>
       <c r="D30" s="21"/>
@@ -1604,7 +1613,7 @@
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B31" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" s="20"/>
       <c r="D31" s="21"/>
@@ -1618,7 +1627,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" s="20"/>
       <c r="D32" s="21"/>
@@ -1632,7 +1641,7 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="20"/>
       <c r="D33" s="21"/>
@@ -1646,7 +1655,7 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="21"/>
@@ -1660,7 +1669,7 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C35" s="20"/>
       <c r="D35" s="21"/>
@@ -1674,7 +1683,7 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="20"/>
       <c r="D36" s="21"/>
@@ -1687,6 +1696,17 @@
       <c r="I36" s="9"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="7">
+        <v>229</v>
+      </c>
+      <c r="F37" s="7">
+        <v>153</v>
+      </c>
       <c r="I37" s="9"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
@@ -1813,102 +1833,91 @@
       <c r="I78" s="9"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B79" s="10" t="s">
+      <c r="I79" s="9"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B80" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C80" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="D80" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D79" s="10" t="s">
+      <c r="E80" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="I80" s="9"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B81" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="E79" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="I79" s="9"/>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B80" s="23" t="s">
+      <c r="C81" s="23">
+        <v>1</v>
+      </c>
+      <c r="D81" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C80" s="23">
-        <v>1</v>
-      </c>
-      <c r="D80" s="23" t="s">
+      <c r="I81" s="9"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B82" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="I80" s="9"/>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B81" s="36" t="s">
+      <c r="C82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="I82" s="9"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B83" s="24"/>
+      <c r="C83" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-      <c r="I81" s="9"/>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B82" s="24"/>
-      <c r="C82" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D82" s="5" t="s">
+      <c r="E83" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E82" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I82" s="9"/>
-    </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B83" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="I83" s="9"/>
-      <c r="J83" s="9"/>
-      <c r="K83" s="25"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="I84" s="9"/>
       <c r="J84" s="9"/>
       <c r="K84" s="25"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>16</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
-      <c r="H85" s="25"/>
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
       <c r="K85" s="25"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
@@ -1919,10 +1928,10 @@
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" s="14" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
@@ -1932,13 +1941,13 @@
       <c r="K87" s="25"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B88" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C88" s="27"/>
-      <c r="D88" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="B88" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D88" s="7"/>
       <c r="E88" s="7"/>
       <c r="H88" s="25"/>
       <c r="I88" s="9"/>
@@ -1947,10 +1956,12 @@
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B89" s="26" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C89" s="27"/>
-      <c r="D89" s="7"/>
+      <c r="D89" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="E89" s="7"/>
       <c r="H89" s="25"/>
       <c r="I89" s="9"/>
@@ -1958,112 +1969,111 @@
       <c r="K89" s="25"/>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B90" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="C90" s="36"/>
-      <c r="D90" s="36"/>
+      <c r="B90" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C90" s="27"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
       <c r="H90" s="25"/>
       <c r="I90" s="9"/>
       <c r="J90" s="9"/>
       <c r="K90" s="25"/>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B91" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E91" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H91" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="B91" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C91" s="37"/>
+      <c r="D91" s="37"/>
+      <c r="H91" s="25"/>
       <c r="I91" s="9"/>
       <c r="J91" s="9"/>
       <c r="K91" s="25"/>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B92" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D92" s="7"/>
-      <c r="E92" s="7"/>
-      <c r="F92" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G92" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H92" s="7" t="s">
-        <v>66</v>
+      <c r="B92" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G92" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="I92" s="9"/>
       <c r="J92" s="9"/>
+      <c r="K92" s="25"/>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B93" s="36" t="s">
+      <c r="B93" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I93" s="9"/>
+      <c r="J93" s="9"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B94" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="J94" s="9"/>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E95" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C93" s="36"/>
-      <c r="D93" s="36"/>
-      <c r="J93" s="9"/>
-    </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B94" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D94" s="5" t="s">
+      <c r="F95" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E94" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J94" s="9"/>
-    </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B95" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E95" s="7"/>
-      <c r="F95" s="8"/>
       <c r="J95" s="9"/>
-      <c r="K95" s="25"/>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B96" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D96" s="7"/>
+        <v>53</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="E96" s="7"/>
       <c r="F96" s="8"/>
       <c r="J96" s="9"/>
@@ -2071,587 +2081,600 @@
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B97" s="7" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
-      <c r="F97" s="35"/>
+      <c r="F97" s="8"/>
       <c r="J97" s="9"/>
       <c r="K97" s="25"/>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B98" s="7" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
-      <c r="F98" s="8"/>
+      <c r="F98" s="35"/>
       <c r="J98" s="9"/>
       <c r="K98" s="25"/>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B99" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C99" s="7">
-        <v>1</v>
-      </c>
+      <c r="B99" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="8"/>
       <c r="J99" s="9"/>
       <c r="K99" s="25"/>
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B100" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C100" s="7">
         <v>1</v>
       </c>
-      <c r="H100" s="25"/>
-      <c r="I100" s="9"/>
       <c r="J100" s="9"/>
       <c r="K100" s="25"/>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B101" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C101" s="7">
+        <v>1</v>
+      </c>
       <c r="H101" s="25"/>
       <c r="I101" s="9"/>
       <c r="J101" s="9"/>
       <c r="K101" s="25"/>
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B102" s="10" t="s">
+      <c r="H102" s="25"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="9"/>
+      <c r="K102" s="25"/>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B103" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C103" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C102" s="10" t="s">
+      <c r="D103" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D102" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E102" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F102" s="22"/>
-    </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B103" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103" s="23">
+      <c r="E103" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F103" s="22"/>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B104" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C104" s="23">
         <v>1</v>
       </c>
-      <c r="D103" s="23"/>
-    </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B104" s="36" t="s">
+      <c r="D104" s="23"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B105" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C105" s="37"/>
+      <c r="D105" s="37"/>
+      <c r="E105" s="37"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B106" s="24"/>
+      <c r="C106" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D106" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C104" s="36"/>
-      <c r="D104" s="36"/>
-      <c r="E104" s="36"/>
-    </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B105" s="24"/>
-      <c r="C105" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D105" s="5" t="s">
+      <c r="E106" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B106" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E106" s="7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B107" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B108" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>16</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B109" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
     </row>
     <row r="110" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B110" s="14" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B111" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C111" s="27"/>
-      <c r="D111" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E111" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="B111" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B112" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C112" s="27"/>
+      <c r="D112" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B113" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C113" s="27"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B114" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C112" s="27"/>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-    </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B113" s="36" t="s">
+      <c r="C114" s="37"/>
+      <c r="D114" s="37"/>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B115" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C115" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C113" s="36"/>
-      <c r="D113" s="36"/>
-    </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B114" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C114" s="5" t="s">
+      <c r="D115" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="E115" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E114" s="5" t="s">
+      <c r="F115" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G115" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H115" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B116" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D116" s="7"/>
+      <c r="E116" s="7"/>
+      <c r="F116" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G116" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H116" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B117" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F114" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G114" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H114" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B115" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C115" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D115" s="7"/>
-      <c r="E115" s="7"/>
-      <c r="F115" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G115" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H115" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B116" s="36" t="s">
+      <c r="C117" s="37"/>
+      <c r="D117" s="37"/>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B118" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E118" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C116" s="36"/>
-      <c r="D116" s="36"/>
-    </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B117" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D117" s="5" t="s">
+      <c r="F118" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E117" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F117" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B118" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C118" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D118" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E118" s="7"/>
-      <c r="F118" s="8"/>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B119" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E119" s="7"/>
+      <c r="F119" s="8"/>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B120" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C119" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F119" s="8"/>
-    </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B120" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C120" s="7">
-        <v>3</v>
-      </c>
+      <c r="C120" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D120" s="7"/>
+      <c r="E120" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120" s="8"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B121" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C121" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B122" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C122" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B123" s="10" t="s">
+    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B124" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B125" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B126" s="37" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B124" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B125" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C125" s="36"/>
-      <c r="D125" s="36"/>
-    </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B126" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C126" s="13"/>
-      <c r="D126" s="34" t="s">
+      <c r="C126" s="37"/>
+      <c r="D126" s="37"/>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B127" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C127" s="13"/>
+      <c r="D127" s="34" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B127" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="C127" s="36"/>
-      <c r="D127" s="36"/>
     </row>
     <row r="128" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B128" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C128" s="37"/>
+      <c r="D128" s="37"/>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B129" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C129" s="49"/>
+      <c r="D129" s="34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B130" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="C128" s="38"/>
-      <c r="D128" s="34" t="s">
+      <c r="C130" s="49"/>
+      <c r="D130" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B132" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C132" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E132" s="22" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B129" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C129" s="38"/>
-      <c r="D129" s="34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B131" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C131" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E131" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F131" s="22"/>
-    </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B132" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C132" s="23">
+      <c r="F132" s="22"/>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B133" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C133" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B133" s="36" t="s">
+    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B134" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C134" s="37"/>
+      <c r="D134" s="37"/>
+      <c r="E134" s="37"/>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B135" s="24"/>
+      <c r="C135" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D135" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C133" s="36"/>
-      <c r="D133" s="36"/>
-      <c r="E133" s="36"/>
-    </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B134" s="24"/>
-      <c r="C134" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D134" s="5" t="s">
+      <c r="E135" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E134" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B135" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C135" s="7"/>
-      <c r="D135" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E135" s="7"/>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B136" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C136" s="7"/>
-      <c r="D136" s="7"/>
+      <c r="D136" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="E136" s="7"/>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B137" s="14" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C137" s="7"/>
-      <c r="D137" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="D137" s="7"/>
       <c r="E137" s="7"/>
     </row>
     <row r="138" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B138" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C138" s="7"/>
       <c r="D138" s="7" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="E138" s="7"/>
     </row>
     <row r="139" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B139" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C139" s="7"/>
+      <c r="D139" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E139" s="7"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B140" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C140" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D140" s="7"/>
+      <c r="E140" s="7"/>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B141" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="C139" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D139" s="7"/>
-      <c r="E139" s="7"/>
-    </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B140" s="39" t="s">
+      <c r="C141" s="50"/>
+      <c r="D141" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C140" s="39"/>
-      <c r="D140" s="7" t="s">
+      <c r="E141" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B142" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E140" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B141" s="26" t="s">
+      <c r="C142" s="27"/>
+      <c r="D142" s="7"/>
+      <c r="E142" s="7"/>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B143" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C141" s="27"/>
-      <c r="D141" s="7"/>
-      <c r="E141" s="7"/>
-    </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B142" s="36" t="s">
+      <c r="C143" s="37"/>
+      <c r="D143" s="37"/>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B144" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C144" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C142" s="36"/>
-      <c r="D142" s="36"/>
-    </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B143" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C143" s="5" t="s">
+      <c r="D144" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D143" s="5" t="s">
+      <c r="E144" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E143" s="5" t="s">
+      <c r="F144" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G144" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H144" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B145" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D145" s="7"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G145" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H145" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B146" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F143" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G143" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H143" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B144" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C144" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D144" s="7"/>
-      <c r="E144" s="7"/>
-      <c r="F144" s="7" t="s">
+      <c r="C146" s="37"/>
+      <c r="D146" s="37"/>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B147" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D147" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E147" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F147" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B148" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G144" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H144" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B145" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="C145" s="36"/>
-      <c r="D145" s="36"/>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B146" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C146" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D146" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E146" s="5" t="s">
+      <c r="C148" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F146" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B147" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C147" s="7" t="s">
+      <c r="D148" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D147" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E147" s="7"/>
-      <c r="F147" s="8"/>
-    </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B148" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D148" s="7"/>
       <c r="E148" s="7"/>
       <c r="F148" s="8"/>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B149" s="14" t="s">
+    <row r="149" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B149" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7"/>
+      <c r="F149" s="8"/>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B150" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C150" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B151" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C149" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B150" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C150" s="7">
+      <c r="C151" s="7">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="23">
+    <mergeCell ref="B143:D143"/>
+    <mergeCell ref="B146:D146"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B105:E105"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B134:E134"/>
+    <mergeCell ref="B126:D126"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B141:C141"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B82:E82"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C4:F5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B142:D142"/>
-    <mergeCell ref="B145:D145"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B93:D93"/>
-    <mergeCell ref="B104:E104"/>
-    <mergeCell ref="B113:D113"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="B125:D125"/>
-    <mergeCell ref="B127:D127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B140:C140"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2661,16 +2684,16 @@
     <oddFooter>&amp;CPrepared by  Nathan Bunker &amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="78" max="16383" man="1"/>
-    <brk id="101" max="16383" man="1"/>
-    <brk id="130" max="16383" man="1"/>
+    <brk id="79" max="16383" man="1"/>
+    <brk id="102" max="16383" man="1"/>
+    <brk id="131" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -2693,7 +2716,7 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B4&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C4&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 205, 204, 203, 202, 217, 218, 219, 220, 221, 222, 223"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Flu" vaccineIds="2050, 180, 181, 1430, 1440, 179, 200, 201, 185, 205, 204, 203, 202, 217, 218, 219, 220, 221, 222, 223, 229"/&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2705,7 +2728,7 @@
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" s="29" t="str">
         <f>"  &lt;vaccine vaccineName="&amp;CHAR(34)&amp;Schedules!B7&amp;CHAR(34)&amp;" vaccineIds="&amp;CHAR(34)&amp;Schedules!C7&amp;CHAR(34)&amp;"/&gt;"</f>
-        <v xml:space="preserve">  &lt;vaccine vaccineName="Live" vaccineIds="158, 159, 160, 161, 162, 171, 175, 178, 2020"/&gt;</v>
+        <v xml:space="preserve">  &lt;vaccine vaccineName="Live" vaccineIds="180, 187, 203, 204, 220"/&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2734,89 +2757,89 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="str">
-        <f>Schedules!B80</f>
+        <f>Schedules!B81</f>
         <v>P1</v>
       </c>
       <c r="B9" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B80&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C80&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D80&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E79&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B81&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E80&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="season"&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C99&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C85&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C85&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C87&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D87&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E87&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C87&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D87&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E87&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C88&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D88&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E88&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D88&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E88&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E89&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B17" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B18" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B92&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F92&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G92&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H92&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B93&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F93&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G93&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H93&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B19" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B95&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D95&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F95&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B96&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D96&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F96&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E96&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B96&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D96&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F96&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E96&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B97&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D97&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F97&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E97&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B21" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B97&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C97&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D97&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F97&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E97&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B98&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D98&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F98&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E98&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="H1N1" schedule="P1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B98&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D98&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F98&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E98&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B99&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C99&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D99&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F99&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E99&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Season Start" schedule="S1" age="" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
@@ -2828,77 +2851,77 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="str">
-        <f>Schedules!B103</f>
+        <f>Schedules!B104</f>
         <v>S1</v>
       </c>
       <c r="B24" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B103&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E102&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B104&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S1" dose="1" indication="" label="current season"&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B25" s="32" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C121&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C120&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C122&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C121&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="3"/&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B26" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D106&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E106&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="6 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B27" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C107&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C108&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C108&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C109&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E109&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C109&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E109&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C110&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D110&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E110&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C110&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D110&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E110&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C111&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D111&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E111&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D111&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E111&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E112&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D113&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B33" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B115&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C115&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D115&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E115&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F115&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G115&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H115&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B116&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C116&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D116&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E116&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F116&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G116&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H116&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B34" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B118&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D118&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F118&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E118&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B119&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C119&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D119&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F119&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E119&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B35" s="32" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B119&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C119&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D119&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F119&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E119&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B120&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C120&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D120&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F120&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E120&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="DL FLU 2015" age="" reason="" seasonCompleted="Yes"/&gt;</v>
       </c>
     </row>
@@ -2910,110 +2933,110 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="30" t="str">
-        <f>Schedules!B124</f>
+        <f>Schedules!B125</f>
         <v>DL FLU 2015</v>
       </c>
       <c r="B37" s="31" t="str">
-        <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B124&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;decisionLogic name="&amp;CHAR(34)&amp;Schedules!B125&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;decisionLogic name="DL FLU 2015"&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="32" t="str">
-        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B126&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;constant name="&amp;CHAR(34)&amp;Schedules!B127&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;constant name="Valid Vaccine" value="Flu"/&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B128&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D128&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B129&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D129&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="Second Dose Needed" value="S2"/&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="32" t="str">
-        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B129&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D129&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;transition name="&amp;CHAR(34)&amp;Schedules!B130&amp;CHAR(34)&amp;" value="&amp;CHAR(34)&amp;Schedules!D130&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;transition name="No More Doses Needed" value="COMPLETE"/&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B41" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="30" t="str">
-        <f>Schedules!B132</f>
+        <f>Schedules!B133</f>
         <v>S2</v>
       </c>
       <c r="B42" s="31" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B132&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D132&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E131&amp;CHAR(34)&amp;"&gt;"</f>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B133&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C133&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D133&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E132&amp;CHAR(34)&amp;"&gt;"</f>
         <v xml:space="preserve">  &lt;schedule scheduleName="S2" dose="2" indication="" label="2nd seasonal"&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="29" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C150&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C149&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C151&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C150&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="32" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" s="32" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C137&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B46" s="32" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C137&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C138&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E138&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="" interval="1 month" grace=""/&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" s="32" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C138&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E138&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C139&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D139&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E139&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="" interval="2 months" grace=""/&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B48" s="32" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C139&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D139&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E139&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C140&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D140&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E140&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="150 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="32" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D140&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E140&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D141&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E141&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="32" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D141&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D142&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B51" s="32" t="str">
-        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B144&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E144&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F144&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G144&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H144&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;contraindicate vaccineName="&amp;CHAR(34)&amp;Schedules!B145&amp;CHAR(34)&amp;" afterInterval="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D145&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!E145&amp;CHAR(34)&amp;" against=" &amp;CHAR(34)&amp;Schedules!F145&amp;CHAR(34)&amp;" contra="&amp;CHAR(34)&amp;Schedules!G145&amp;CHAR(34)&amp;" allowed="&amp;CHAR(34)&amp;Schedules!H145&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;contraindicate vaccineName="Live" afterInterval="4 weeks" age="" reason="" against="Nasal" contra="Influenza LAIV" allowed="Influenza IIV"/&gt;</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B52" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B147&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C147&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D147&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F147&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H147&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E147&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B148&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C148&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D148&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F148&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H148&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E148&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Nasal" schedule="INVALID" age="2 years" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B53" s="33" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B148&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C148&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D148&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F148&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H148&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E148&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B149&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C149&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D149&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F149&amp;CHAR(34)&amp;" minInterval="&amp;CHAR(34)&amp;Schedules!H149&amp;CHAR(34)&amp;" seasonCompleted="&amp;CHAR(34)&amp;Schedules!E149&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="Flu" schedule="COMPLETE" age="" reason="" minInterval="" seasonCompleted=""/&gt;</v>
       </c>
     </row>

</xml_diff>